<commit_message>
Increased amount of test data
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1603.6.microbial.xlsx
+++ b/tests/fixtures/orderforms/1603.6.microbial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B8B474A2-F4D6-E846-BB57-ED17A8BEEC20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A63A28F6-84E2-DF44-AF48-9B3942D5A569}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1540" windowWidth="42200" windowHeight="8180" tabRatio="593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" tabRatio="593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order form" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="340">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -359,6 +359,7 @@
         <i/>
         <sz val="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Other</t>
@@ -368,6 +369,7 @@
         <b/>
         <sz val="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> please specify in Comment field)</t>
@@ -888,6 +890,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Important: </t>
     </r>
@@ -910,6 +913,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Options available in drop down list.
 </t>
@@ -924,6 +928,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Delivery data mode. Options available in drop down list.
 </t>
@@ -938,6 +943,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">States the application of the order. Options available in drop down list.
 </t>
@@ -952,6 +958,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Options available in drop down list. Must be in format custXXX.
 </t>
@@ -1021,6 +1028,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>order form</t>
     </r>
@@ -1043,6 +1051,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>application tag</t>
     </r>
@@ -1064,6 +1073,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Options available in drop down list. If "other" please specify in comment field.</t>
     </r>
@@ -1077,6 +1087,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Options available in drop down list. If other, please specify in comment field.</t>
     </r>
@@ -1098,6 +1109,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1115,6 +1127,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>standard</t>
     </r>
@@ -1167,6 +1180,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Please note that it's not possible to exclude individual samples when ordering MWXNXTR002.</t>
     </r>
@@ -1225,6 +1239,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Use accession no. From NCBI.</t>
     </r>
@@ -1315,6 +1330,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>all the fields</t>
     </r>
@@ -1332,6 +1348,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>these fields are required</t>
     </r>
@@ -1349,6 +1366,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>sample name</t>
     </r>
@@ -1366,6 +1384,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>drop down lists</t>
     </r>
@@ -1383,6 +1402,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>order form</t>
     </r>
@@ -1397,15 +1417,6 @@
     </r>
   </si>
   <si>
-    <t>Jag</t>
-  </si>
-  <si>
-    <t>testar</t>
-  </si>
-  <si>
-    <t>lite</t>
-  </si>
-  <si>
     <t>M.upium</t>
   </si>
   <si>
@@ -1418,10 +1429,34 @@
     <t>NC_333</t>
   </si>
   <si>
-    <t>hej</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>name of plate</t>
+  </si>
+  <si>
+    <t>plate comment</t>
+  </si>
+  <si>
+    <t>NC_444</t>
+  </si>
+  <si>
+    <t>NC_555</t>
+  </si>
+  <si>
+    <t>optional comment</t>
+  </si>
+  <si>
+    <t>all-fields</t>
+  </si>
+  <si>
+    <t>required-fields</t>
+  </si>
+  <si>
+    <t>plate-fields</t>
+  </si>
+  <si>
+    <t>other-species-fields</t>
+  </si>
+  <si>
+    <t>optional-fields</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1490,12 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1474,19 +1511,23 @@
     <font>
       <sz val="9"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1499,49 +1540,58 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1549,12 +1599,14 @@
       <sz val="12"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1562,18 +1614,21 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1581,11 +1636,13 @@
       <u/>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1593,18 +1650,21 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFC83264"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1612,48 +1672,57 @@
       <i/>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF606060"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC83264"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1666,47 +1735,56 @@
       <sz val="6"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2263,7 +2341,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2570,11 +2648,7 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="42" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2591,7 +2665,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="134" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2600,21 +2674,21 @@
     <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="37" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="15" xfId="224" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="9" borderId="15" xfId="224" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2622,7 +2696,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="42" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2634,7 +2708,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2655,7 +2729,7 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2675,6 +2749,10 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="305">
@@ -3540,8 +3618,8 @@
   </sheetPr>
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -3882,11 +3960,11 @@
       <c r="V12" s="54"/>
     </row>
     <row r="13" spans="1:22" ht="24" customHeight="1">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="116" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
@@ -3932,34 +4010,34 @@
       <c r="V14" s="57"/>
     </row>
     <row r="15" spans="1:22" s="7" customFormat="1" ht="22">
-      <c r="A15" s="149" t="s">
+      <c r="A15" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="150"/>
-      <c r="F15" s="150"/>
-      <c r="G15" s="150"/>
-      <c r="H15" s="150"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="151"/>
+      <c r="B15" s="149"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="149"/>
+      <c r="E15" s="149"/>
+      <c r="F15" s="149"/>
+      <c r="G15" s="149"/>
+      <c r="H15" s="149"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="149"/>
+      <c r="K15" s="150"/>
       <c r="L15" s="74"/>
-      <c r="M15" s="153" t="s">
+      <c r="M15" s="152" t="s">
         <v>108</v>
       </c>
-      <c r="N15" s="154"/>
-      <c r="O15" s="137"/>
+      <c r="N15" s="153"/>
+      <c r="O15" s="136"/>
       <c r="P15" s="83" t="s">
         <v>308</v>
       </c>
       <c r="Q15" s="60"/>
-      <c r="R15" s="149" t="s">
+      <c r="R15" s="148" t="s">
         <v>106</v>
       </c>
-      <c r="S15" s="150"/>
-      <c r="T15" s="152"/>
+      <c r="S15" s="149"/>
+      <c r="T15" s="151"/>
       <c r="U15" s="23"/>
       <c r="V15" s="23"/>
     </row>
@@ -4030,7 +4108,7 @@
       <c r="N17" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="138"/>
+      <c r="O17" s="137"/>
       <c r="P17" s="20" t="s">
         <v>309</v>
       </c>
@@ -4116,7 +4194,7 @@
       <c r="N19" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="O19" s="137"/>
+      <c r="O19" s="136"/>
       <c r="P19" s="17" t="s">
         <v>303</v>
       </c>
@@ -4161,15 +4239,15 @@
       <c r="U20" s="25"/>
       <c r="V20" s="27"/>
     </row>
-    <row r="21" spans="1:22" s="116" customFormat="1" ht="13" customHeight="1">
-      <c r="A21" s="143" t="s">
-        <v>326</v>
+    <row r="21" spans="1:22" s="115" customFormat="1" ht="13" customHeight="1">
+      <c r="A21" s="154" t="s">
+        <v>335</v>
       </c>
       <c r="B21" s="107" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C21" s="107" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D21" s="108" t="s">
         <v>20</v>
@@ -4196,34 +4274,40 @@
         <v>21</v>
       </c>
       <c r="L21" s="111"/>
-      <c r="M21" s="112" t="s">
-        <v>333</v>
-      </c>
-      <c r="N21" s="113" t="s">
-        <v>136</v>
-      </c>
-      <c r="O21" s="139"/>
-      <c r="P21" s="144"/>
-      <c r="Q21" s="114"/>
-      <c r="R21" s="115">
-        <v>1</v>
-      </c>
-      <c r="S21" s="115"/>
-      <c r="T21" s="144"/>
-      <c r="U21" s="114"/>
+      <c r="M21" s="154" t="s">
+        <v>330</v>
+      </c>
+      <c r="N21" s="112" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" s="138"/>
+      <c r="P21" s="143" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q21" s="113"/>
+      <c r="R21" s="114">
+        <v>101</v>
+      </c>
+      <c r="S21" s="114">
+        <v>102</v>
+      </c>
+      <c r="T21" s="154" t="s">
+        <v>331</v>
+      </c>
+      <c r="U21" s="113"/>
       <c r="V21" s="110" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A22" s="143" t="s">
-        <v>327</v>
+      <c r="A22" s="154" t="s">
+        <v>336</v>
       </c>
       <c r="B22" s="107" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C22" s="107" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D22" s="108" t="s">
         <v>20</v>
@@ -4244,42 +4328,34 @@
         <v>302</v>
       </c>
       <c r="J22" s="107" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="K22" s="107" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="90"/>
-      <c r="M22" s="96" t="s">
-        <v>333</v>
-      </c>
-      <c r="N22" s="97" t="s">
-        <v>140</v>
-      </c>
-      <c r="O22" s="140"/>
-      <c r="P22" s="145" t="s">
-        <v>329</v>
-      </c>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="139"/>
+      <c r="P22" s="144"/>
       <c r="Q22" s="93"/>
       <c r="R22" s="94"/>
-      <c r="S22" s="94">
-        <v>2</v>
-      </c>
-      <c r="T22" s="145"/>
+      <c r="S22" s="94"/>
+      <c r="T22" s="144"/>
       <c r="U22" s="93"/>
       <c r="V22" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A23" s="143" t="s">
-        <v>328</v>
+      <c r="A23" s="154" t="s">
+        <v>337</v>
       </c>
       <c r="B23" s="107" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C23" s="107" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D23" s="108" t="s">
         <v>20</v>
@@ -4306,79 +4382,128 @@
         <v>21</v>
       </c>
       <c r="L23" s="90"/>
-      <c r="M23" s="96" t="s">
-        <v>333</v>
+      <c r="M23" s="155" t="s">
+        <v>330</v>
       </c>
       <c r="N23" s="97" t="s">
-        <v>141</v>
-      </c>
-      <c r="O23" s="140"/>
-      <c r="P23" s="145"/>
+        <v>109</v>
+      </c>
+      <c r="O23" s="139"/>
+      <c r="P23" s="144"/>
       <c r="Q23" s="93"/>
       <c r="R23" s="94"/>
       <c r="S23" s="94"/>
-      <c r="T23" s="145" t="s">
-        <v>334</v>
-      </c>
+      <c r="T23" s="144"/>
       <c r="U23" s="93"/>
       <c r="V23" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A24" s="143"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="107"/>
-      <c r="K24" s="107"/>
+      <c r="A24" s="154" t="s">
+        <v>338</v>
+      </c>
+      <c r="B24" s="107" t="s">
+        <v>301</v>
+      </c>
+      <c r="C24" s="107" t="s">
+        <v>332</v>
+      </c>
+      <c r="D24" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="109" t="s">
+        <v>300</v>
+      </c>
+      <c r="F24" s="110" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="107" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="107" t="s">
+        <v>302</v>
+      </c>
+      <c r="J24" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="107" t="s">
+        <v>21</v>
+      </c>
       <c r="L24" s="90"/>
       <c r="M24" s="96"/>
-      <c r="N24" s="98"/>
-      <c r="O24" s="141"/>
-      <c r="P24" s="145"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="139"/>
+      <c r="P24" s="143" t="s">
+        <v>326</v>
+      </c>
       <c r="Q24" s="93"/>
       <c r="R24" s="94"/>
       <c r="S24" s="94"/>
-      <c r="T24" s="145"/>
+      <c r="T24" s="144"/>
       <c r="U24" s="93"/>
       <c r="V24" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A25" s="143"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="107"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="107"/>
-      <c r="K25" s="107"/>
+      <c r="A25" s="154" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" s="107" t="s">
+        <v>310</v>
+      </c>
+      <c r="C25" s="107" t="s">
+        <v>333</v>
+      </c>
+      <c r="D25" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="109" t="s">
+        <v>300</v>
+      </c>
+      <c r="F25" s="110" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="107" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="107" t="s">
+        <v>302</v>
+      </c>
+      <c r="J25" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="107" t="s">
+        <v>21</v>
+      </c>
       <c r="L25" s="90"/>
       <c r="M25" s="96"/>
       <c r="N25" s="97"/>
-      <c r="O25" s="140"/>
-      <c r="P25" s="145"/>
+      <c r="O25" s="139"/>
+      <c r="P25" s="143"/>
       <c r="Q25" s="93"/>
-      <c r="R25" s="94"/>
-      <c r="S25" s="94"/>
-      <c r="T25" s="145"/>
+      <c r="R25" s="154">
+        <v>201</v>
+      </c>
+      <c r="S25" s="94">
+        <v>202</v>
+      </c>
+      <c r="T25" s="154" t="s">
+        <v>334</v>
+      </c>
       <c r="U25" s="93"/>
       <c r="V25" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A26" s="143"/>
       <c r="B26" s="107"/>
       <c r="C26" s="107"/>
       <c r="D26" s="108"/>
@@ -4392,19 +4517,19 @@
       <c r="L26" s="90"/>
       <c r="M26" s="96"/>
       <c r="N26" s="97"/>
-      <c r="O26" s="140"/>
-      <c r="P26" s="145"/>
+      <c r="O26" s="139"/>
+      <c r="P26" s="144"/>
       <c r="Q26" s="93"/>
       <c r="R26" s="94"/>
       <c r="S26" s="94"/>
-      <c r="T26" s="145"/>
+      <c r="T26" s="144"/>
       <c r="U26" s="93"/>
       <c r="V26" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A27" s="143"/>
+      <c r="A27" s="142"/>
       <c r="B27" s="107"/>
       <c r="C27" s="107"/>
       <c r="D27" s="108"/>
@@ -4418,19 +4543,19 @@
       <c r="L27" s="77"/>
       <c r="M27" s="85"/>
       <c r="N27" s="98"/>
-      <c r="O27" s="141"/>
-      <c r="P27" s="146"/>
+      <c r="O27" s="140"/>
+      <c r="P27" s="145"/>
       <c r="Q27" s="93"/>
       <c r="R27" s="72"/>
       <c r="S27" s="72"/>
-      <c r="T27" s="147"/>
+      <c r="T27" s="146"/>
       <c r="U27" s="93"/>
       <c r="V27" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:22" s="95" customFormat="1" ht="11" customHeight="1">
-      <c r="A28" s="143"/>
+      <c r="A28" s="142"/>
       <c r="B28" s="107"/>
       <c r="C28" s="107"/>
       <c r="D28" s="108"/>
@@ -4444,19 +4569,19 @@
       <c r="L28" s="77"/>
       <c r="M28" s="85"/>
       <c r="N28" s="97"/>
-      <c r="O28" s="140"/>
-      <c r="P28" s="146"/>
+      <c r="O28" s="139"/>
+      <c r="P28" s="145"/>
       <c r="Q28" s="93"/>
       <c r="R28" s="72"/>
       <c r="S28" s="72"/>
-      <c r="T28" s="147"/>
+      <c r="T28" s="146"/>
       <c r="U28" s="93"/>
       <c r="V28" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="11" customHeight="1">
-      <c r="A29" s="143"/>
+      <c r="A29" s="142"/>
       <c r="B29" s="107"/>
       <c r="C29" s="107"/>
       <c r="D29" s="108"/>
@@ -4470,19 +4595,19 @@
       <c r="L29" s="90"/>
       <c r="M29" s="91"/>
       <c r="N29" s="92"/>
-      <c r="O29" s="141"/>
-      <c r="P29" s="145"/>
+      <c r="O29" s="140"/>
+      <c r="P29" s="144"/>
       <c r="Q29" s="93"/>
       <c r="R29" s="94"/>
       <c r="S29" s="94"/>
-      <c r="T29" s="145"/>
+      <c r="T29" s="144"/>
       <c r="U29" s="93"/>
       <c r="V29" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="143"/>
+      <c r="A30" s="142"/>
       <c r="B30" s="107"/>
       <c r="C30" s="107"/>
       <c r="D30" s="108"/>
@@ -4496,19 +4621,19 @@
       <c r="L30" s="90"/>
       <c r="M30" s="96"/>
       <c r="N30" s="97"/>
-      <c r="O30" s="140"/>
-      <c r="P30" s="145"/>
+      <c r="O30" s="139"/>
+      <c r="P30" s="144"/>
       <c r="Q30" s="93"/>
       <c r="R30" s="94"/>
       <c r="S30" s="94"/>
-      <c r="T30" s="145"/>
+      <c r="T30" s="144"/>
       <c r="U30" s="93"/>
       <c r="V30" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="143"/>
+      <c r="A31" s="142"/>
       <c r="B31" s="107"/>
       <c r="C31" s="107"/>
       <c r="D31" s="108"/>
@@ -4522,19 +4647,19 @@
       <c r="L31" s="90"/>
       <c r="M31" s="96"/>
       <c r="N31" s="97"/>
-      <c r="O31" s="140"/>
-      <c r="P31" s="145"/>
+      <c r="O31" s="139"/>
+      <c r="P31" s="144"/>
       <c r="Q31" s="93"/>
       <c r="R31" s="94"/>
       <c r="S31" s="94"/>
-      <c r="T31" s="145"/>
+      <c r="T31" s="144"/>
       <c r="U31" s="93"/>
       <c r="V31" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="143"/>
+      <c r="A32" s="142"/>
       <c r="B32" s="107"/>
       <c r="C32" s="107"/>
       <c r="D32" s="108"/>
@@ -4548,19 +4673,19 @@
       <c r="L32" s="90"/>
       <c r="M32" s="96"/>
       <c r="N32" s="98"/>
-      <c r="O32" s="141"/>
-      <c r="P32" s="145"/>
+      <c r="O32" s="140"/>
+      <c r="P32" s="144"/>
       <c r="Q32" s="93"/>
       <c r="R32" s="94"/>
       <c r="S32" s="94"/>
-      <c r="T32" s="145"/>
+      <c r="T32" s="144"/>
       <c r="U32" s="93"/>
       <c r="V32" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A33" s="143"/>
+      <c r="A33" s="142"/>
       <c r="B33" s="107"/>
       <c r="C33" s="107"/>
       <c r="D33" s="108"/>
@@ -4574,19 +4699,19 @@
       <c r="L33" s="90"/>
       <c r="M33" s="96"/>
       <c r="N33" s="97"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="145"/>
+      <c r="O33" s="139"/>
+      <c r="P33" s="144"/>
       <c r="Q33" s="93"/>
       <c r="R33" s="94"/>
       <c r="S33" s="94"/>
-      <c r="T33" s="145"/>
+      <c r="T33" s="144"/>
       <c r="U33" s="93"/>
       <c r="V33" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A34" s="143"/>
+      <c r="A34" s="142"/>
       <c r="B34" s="107"/>
       <c r="C34" s="107"/>
       <c r="D34" s="108"/>
@@ -4600,19 +4725,19 @@
       <c r="L34" s="90"/>
       <c r="M34" s="96"/>
       <c r="N34" s="97"/>
-      <c r="O34" s="140"/>
-      <c r="P34" s="145"/>
+      <c r="O34" s="139"/>
+      <c r="P34" s="144"/>
       <c r="Q34" s="93"/>
       <c r="R34" s="94"/>
       <c r="S34" s="94"/>
-      <c r="T34" s="145"/>
+      <c r="T34" s="144"/>
       <c r="U34" s="93"/>
       <c r="V34" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A35" s="143"/>
+      <c r="A35" s="142"/>
       <c r="B35" s="107"/>
       <c r="C35" s="107"/>
       <c r="D35" s="108"/>
@@ -4626,19 +4751,19 @@
       <c r="L35" s="77"/>
       <c r="M35" s="85"/>
       <c r="N35" s="98"/>
-      <c r="O35" s="141"/>
-      <c r="P35" s="146"/>
+      <c r="O35" s="140"/>
+      <c r="P35" s="145"/>
       <c r="Q35" s="93"/>
       <c r="R35" s="72"/>
       <c r="S35" s="72"/>
-      <c r="T35" s="147"/>
+      <c r="T35" s="146"/>
       <c r="U35" s="93"/>
       <c r="V35" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A36" s="143"/>
+      <c r="A36" s="142"/>
       <c r="B36" s="107"/>
       <c r="C36" s="107"/>
       <c r="D36" s="108"/>
@@ -4652,19 +4777,19 @@
       <c r="L36" s="77"/>
       <c r="M36" s="85"/>
       <c r="N36" s="97"/>
-      <c r="O36" s="140"/>
-      <c r="P36" s="146"/>
+      <c r="O36" s="139"/>
+      <c r="P36" s="145"/>
       <c r="Q36" s="93"/>
       <c r="R36" s="72"/>
       <c r="S36" s="72"/>
-      <c r="T36" s="147"/>
+      <c r="T36" s="146"/>
       <c r="U36" s="93"/>
       <c r="V36" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A37" s="143"/>
+      <c r="A37" s="142"/>
       <c r="B37" s="107"/>
       <c r="C37" s="107"/>
       <c r="D37" s="108"/>
@@ -4678,19 +4803,19 @@
       <c r="L37" s="90"/>
       <c r="M37" s="91"/>
       <c r="N37" s="92"/>
-      <c r="O37" s="141"/>
-      <c r="P37" s="145"/>
+      <c r="O37" s="140"/>
+      <c r="P37" s="144"/>
       <c r="Q37" s="93"/>
       <c r="R37" s="94"/>
       <c r="S37" s="94"/>
-      <c r="T37" s="145"/>
+      <c r="T37" s="144"/>
       <c r="U37" s="93"/>
       <c r="V37" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A38" s="143"/>
+      <c r="A38" s="142"/>
       <c r="B38" s="107"/>
       <c r="C38" s="107"/>
       <c r="D38" s="108"/>
@@ -4704,19 +4829,19 @@
       <c r="L38" s="90"/>
       <c r="M38" s="96"/>
       <c r="N38" s="97"/>
-      <c r="O38" s="140"/>
-      <c r="P38" s="145"/>
+      <c r="O38" s="139"/>
+      <c r="P38" s="144"/>
       <c r="Q38" s="93"/>
       <c r="R38" s="94"/>
       <c r="S38" s="94"/>
-      <c r="T38" s="145"/>
+      <c r="T38" s="144"/>
       <c r="U38" s="93"/>
       <c r="V38" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A39" s="143"/>
+      <c r="A39" s="142"/>
       <c r="B39" s="107"/>
       <c r="C39" s="107"/>
       <c r="D39" s="108"/>
@@ -4730,19 +4855,19 @@
       <c r="L39" s="90"/>
       <c r="M39" s="96"/>
       <c r="N39" s="97"/>
-      <c r="O39" s="140"/>
-      <c r="P39" s="145"/>
+      <c r="O39" s="139"/>
+      <c r="P39" s="144"/>
       <c r="Q39" s="93"/>
       <c r="R39" s="94"/>
       <c r="S39" s="94"/>
-      <c r="T39" s="145"/>
+      <c r="T39" s="144"/>
       <c r="U39" s="93"/>
       <c r="V39" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A40" s="143"/>
+      <c r="A40" s="142"/>
       <c r="B40" s="107"/>
       <c r="C40" s="107"/>
       <c r="D40" s="108"/>
@@ -4756,19 +4881,19 @@
       <c r="L40" s="90"/>
       <c r="M40" s="96"/>
       <c r="N40" s="98"/>
-      <c r="O40" s="141"/>
-      <c r="P40" s="145"/>
+      <c r="O40" s="140"/>
+      <c r="P40" s="144"/>
       <c r="Q40" s="93"/>
       <c r="R40" s="94"/>
       <c r="S40" s="94"/>
-      <c r="T40" s="145"/>
+      <c r="T40" s="144"/>
       <c r="U40" s="93"/>
       <c r="V40" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:22" s="10" customFormat="1" ht="11">
-      <c r="A41" s="143"/>
+      <c r="A41" s="142"/>
       <c r="B41" s="107"/>
       <c r="C41" s="107"/>
       <c r="D41" s="108"/>
@@ -4782,19 +4907,19 @@
       <c r="L41" s="90"/>
       <c r="M41" s="96"/>
       <c r="N41" s="97"/>
-      <c r="O41" s="140"/>
-      <c r="P41" s="145"/>
+      <c r="O41" s="139"/>
+      <c r="P41" s="144"/>
       <c r="Q41" s="93"/>
       <c r="R41" s="94"/>
       <c r="S41" s="94"/>
-      <c r="T41" s="145"/>
+      <c r="T41" s="144"/>
       <c r="U41" s="93"/>
       <c r="V41" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="6" customFormat="1">
-      <c r="A42" s="143"/>
+      <c r="A42" s="142"/>
       <c r="B42" s="107"/>
       <c r="C42" s="107"/>
       <c r="D42" s="108"/>
@@ -4808,19 +4933,19 @@
       <c r="L42" s="90"/>
       <c r="M42" s="96"/>
       <c r="N42" s="97"/>
-      <c r="O42" s="140"/>
-      <c r="P42" s="145"/>
+      <c r="O42" s="139"/>
+      <c r="P42" s="144"/>
       <c r="Q42" s="93"/>
       <c r="R42" s="94"/>
       <c r="S42" s="94"/>
-      <c r="T42" s="145"/>
+      <c r="T42" s="144"/>
       <c r="U42" s="93"/>
       <c r="V42" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="6" customFormat="1">
-      <c r="A43" s="143"/>
+      <c r="A43" s="142"/>
       <c r="B43" s="107"/>
       <c r="C43" s="107"/>
       <c r="D43" s="108"/>
@@ -4834,19 +4959,19 @@
       <c r="L43" s="77"/>
       <c r="M43" s="85"/>
       <c r="N43" s="98"/>
-      <c r="O43" s="141"/>
-      <c r="P43" s="146"/>
+      <c r="O43" s="140"/>
+      <c r="P43" s="145"/>
       <c r="Q43" s="93"/>
       <c r="R43" s="72"/>
       <c r="S43" s="72"/>
-      <c r="T43" s="147"/>
+      <c r="T43" s="146"/>
       <c r="U43" s="93"/>
       <c r="V43" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:22" s="6" customFormat="1">
-      <c r="A44" s="143"/>
+      <c r="A44" s="142"/>
       <c r="B44" s="107"/>
       <c r="C44" s="107"/>
       <c r="D44" s="108"/>
@@ -4860,19 +4985,19 @@
       <c r="L44" s="77"/>
       <c r="M44" s="85"/>
       <c r="N44" s="97"/>
-      <c r="O44" s="140"/>
-      <c r="P44" s="146"/>
+      <c r="O44" s="139"/>
+      <c r="P44" s="145"/>
       <c r="Q44" s="93"/>
       <c r="R44" s="72"/>
       <c r="S44" s="72"/>
-      <c r="T44" s="147"/>
+      <c r="T44" s="146"/>
       <c r="U44" s="93"/>
       <c r="V44" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:22">
-      <c r="A45" s="143"/>
+      <c r="A45" s="142"/>
       <c r="B45" s="107"/>
       <c r="C45" s="107"/>
       <c r="D45" s="108"/>
@@ -4886,19 +5011,19 @@
       <c r="L45" s="90"/>
       <c r="M45" s="91"/>
       <c r="N45" s="92"/>
-      <c r="O45" s="141"/>
-      <c r="P45" s="145"/>
+      <c r="O45" s="140"/>
+      <c r="P45" s="144"/>
       <c r="Q45" s="93"/>
       <c r="R45" s="94"/>
       <c r="S45" s="94"/>
-      <c r="T45" s="145"/>
+      <c r="T45" s="144"/>
       <c r="U45" s="93"/>
       <c r="V45" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:22">
-      <c r="A46" s="143"/>
+      <c r="A46" s="142"/>
       <c r="B46" s="107"/>
       <c r="C46" s="107"/>
       <c r="D46" s="108"/>
@@ -4912,19 +5037,19 @@
       <c r="L46" s="90"/>
       <c r="M46" s="96"/>
       <c r="N46" s="97"/>
-      <c r="O46" s="140"/>
-      <c r="P46" s="145"/>
+      <c r="O46" s="139"/>
+      <c r="P46" s="144"/>
       <c r="Q46" s="93"/>
       <c r="R46" s="94"/>
       <c r="S46" s="94"/>
-      <c r="T46" s="145"/>
+      <c r="T46" s="144"/>
       <c r="U46" s="93"/>
       <c r="V46" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:22">
-      <c r="A47" s="143"/>
+      <c r="A47" s="142"/>
       <c r="B47" s="107"/>
       <c r="C47" s="107"/>
       <c r="D47" s="108"/>
@@ -4938,19 +5063,19 @@
       <c r="L47" s="90"/>
       <c r="M47" s="96"/>
       <c r="N47" s="97"/>
-      <c r="O47" s="140"/>
-      <c r="P47" s="145"/>
+      <c r="O47" s="139"/>
+      <c r="P47" s="144"/>
       <c r="Q47" s="93"/>
       <c r="R47" s="94"/>
       <c r="S47" s="94"/>
-      <c r="T47" s="145"/>
+      <c r="T47" s="144"/>
       <c r="U47" s="93"/>
       <c r="V47" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:22">
-      <c r="A48" s="143"/>
+      <c r="A48" s="142"/>
       <c r="B48" s="107"/>
       <c r="C48" s="107"/>
       <c r="D48" s="108"/>
@@ -4964,19 +5089,19 @@
       <c r="L48" s="90"/>
       <c r="M48" s="96"/>
       <c r="N48" s="98"/>
-      <c r="O48" s="141"/>
-      <c r="P48" s="145"/>
+      <c r="O48" s="140"/>
+      <c r="P48" s="144"/>
       <c r="Q48" s="93"/>
       <c r="R48" s="94"/>
       <c r="S48" s="94"/>
-      <c r="T48" s="145"/>
+      <c r="T48" s="144"/>
       <c r="U48" s="93"/>
       <c r="V48" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:22">
-      <c r="A49" s="143"/>
+      <c r="A49" s="142"/>
       <c r="B49" s="107"/>
       <c r="C49" s="107"/>
       <c r="D49" s="108"/>
@@ -4990,19 +5115,19 @@
       <c r="L49" s="90"/>
       <c r="M49" s="96"/>
       <c r="N49" s="97"/>
-      <c r="O49" s="140"/>
-      <c r="P49" s="145"/>
+      <c r="O49" s="139"/>
+      <c r="P49" s="144"/>
       <c r="Q49" s="93"/>
       <c r="R49" s="94"/>
       <c r="S49" s="94"/>
-      <c r="T49" s="145"/>
+      <c r="T49" s="144"/>
       <c r="U49" s="93"/>
       <c r="V49" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:22">
-      <c r="A50" s="143"/>
+      <c r="A50" s="142"/>
       <c r="B50" s="107"/>
       <c r="C50" s="107"/>
       <c r="D50" s="108"/>
@@ -5016,19 +5141,19 @@
       <c r="L50" s="90"/>
       <c r="M50" s="96"/>
       <c r="N50" s="97"/>
-      <c r="O50" s="140"/>
-      <c r="P50" s="145"/>
+      <c r="O50" s="139"/>
+      <c r="P50" s="144"/>
       <c r="Q50" s="93"/>
       <c r="R50" s="94"/>
       <c r="S50" s="94"/>
-      <c r="T50" s="145"/>
+      <c r="T50" s="144"/>
       <c r="U50" s="93"/>
       <c r="V50" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:22">
-      <c r="A51" s="143"/>
+      <c r="A51" s="142"/>
       <c r="B51" s="107"/>
       <c r="C51" s="107"/>
       <c r="D51" s="108"/>
@@ -5042,19 +5167,19 @@
       <c r="L51" s="77"/>
       <c r="M51" s="85"/>
       <c r="N51" s="98"/>
-      <c r="O51" s="141"/>
-      <c r="P51" s="146"/>
+      <c r="O51" s="140"/>
+      <c r="P51" s="145"/>
       <c r="Q51" s="93"/>
       <c r="R51" s="72"/>
       <c r="S51" s="72"/>
-      <c r="T51" s="147"/>
+      <c r="T51" s="146"/>
       <c r="U51" s="93"/>
       <c r="V51" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:22">
-      <c r="A52" s="143"/>
+      <c r="A52" s="142"/>
       <c r="B52" s="107"/>
       <c r="C52" s="107"/>
       <c r="D52" s="108"/>
@@ -5068,19 +5193,19 @@
       <c r="L52" s="77"/>
       <c r="M52" s="85"/>
       <c r="N52" s="97"/>
-      <c r="O52" s="140"/>
-      <c r="P52" s="146"/>
+      <c r="O52" s="139"/>
+      <c r="P52" s="145"/>
       <c r="Q52" s="93"/>
       <c r="R52" s="72"/>
       <c r="S52" s="72"/>
-      <c r="T52" s="147"/>
+      <c r="T52" s="146"/>
       <c r="U52" s="93"/>
       <c r="V52" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:22">
-      <c r="A53" s="143"/>
+      <c r="A53" s="142"/>
       <c r="B53" s="107"/>
       <c r="C53" s="107"/>
       <c r="D53" s="108"/>
@@ -5094,19 +5219,19 @@
       <c r="L53" s="90"/>
       <c r="M53" s="91"/>
       <c r="N53" s="92"/>
-      <c r="O53" s="141"/>
-      <c r="P53" s="145"/>
+      <c r="O53" s="140"/>
+      <c r="P53" s="144"/>
       <c r="Q53" s="93"/>
       <c r="R53" s="94"/>
       <c r="S53" s="94"/>
-      <c r="T53" s="145"/>
+      <c r="T53" s="144"/>
       <c r="U53" s="93"/>
       <c r="V53" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:22">
-      <c r="A54" s="143"/>
+      <c r="A54" s="142"/>
       <c r="B54" s="107"/>
       <c r="C54" s="107"/>
       <c r="D54" s="108"/>
@@ -5120,19 +5245,19 @@
       <c r="L54" s="90"/>
       <c r="M54" s="96"/>
       <c r="N54" s="97"/>
-      <c r="O54" s="140"/>
-      <c r="P54" s="145"/>
+      <c r="O54" s="139"/>
+      <c r="P54" s="144"/>
       <c r="Q54" s="93"/>
       <c r="R54" s="94"/>
       <c r="S54" s="94"/>
-      <c r="T54" s="145"/>
+      <c r="T54" s="144"/>
       <c r="U54" s="93"/>
       <c r="V54" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:22">
-      <c r="A55" s="143"/>
+      <c r="A55" s="142"/>
       <c r="B55" s="107"/>
       <c r="C55" s="107"/>
       <c r="D55" s="108"/>
@@ -5146,19 +5271,19 @@
       <c r="L55" s="90"/>
       <c r="M55" s="96"/>
       <c r="N55" s="97"/>
-      <c r="O55" s="140"/>
-      <c r="P55" s="145"/>
+      <c r="O55" s="139"/>
+      <c r="P55" s="144"/>
       <c r="Q55" s="93"/>
       <c r="R55" s="94"/>
       <c r="S55" s="94"/>
-      <c r="T55" s="145"/>
+      <c r="T55" s="144"/>
       <c r="U55" s="93"/>
       <c r="V55" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A56" s="143"/>
+      <c r="A56" s="142"/>
       <c r="B56" s="107"/>
       <c r="C56" s="107"/>
       <c r="D56" s="108"/>
@@ -5172,19 +5297,19 @@
       <c r="L56" s="90"/>
       <c r="M56" s="96"/>
       <c r="N56" s="98"/>
-      <c r="O56" s="141"/>
-      <c r="P56" s="145"/>
+      <c r="O56" s="140"/>
+      <c r="P56" s="144"/>
       <c r="Q56" s="93"/>
       <c r="R56" s="94"/>
       <c r="S56" s="94"/>
-      <c r="T56" s="145"/>
+      <c r="T56" s="144"/>
       <c r="U56" s="93"/>
       <c r="V56" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A57" s="143"/>
+      <c r="A57" s="142"/>
       <c r="B57" s="107"/>
       <c r="C57" s="107"/>
       <c r="D57" s="108"/>
@@ -5198,19 +5323,19 @@
       <c r="L57" s="90"/>
       <c r="M57" s="96"/>
       <c r="N57" s="97"/>
-      <c r="O57" s="140"/>
-      <c r="P57" s="145"/>
+      <c r="O57" s="139"/>
+      <c r="P57" s="144"/>
       <c r="Q57" s="93"/>
       <c r="R57" s="94"/>
       <c r="S57" s="94"/>
-      <c r="T57" s="145"/>
+      <c r="T57" s="144"/>
       <c r="U57" s="93"/>
       <c r="V57" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A58" s="143"/>
+      <c r="A58" s="142"/>
       <c r="B58" s="107"/>
       <c r="C58" s="107"/>
       <c r="D58" s="108"/>
@@ -5224,19 +5349,19 @@
       <c r="L58" s="90"/>
       <c r="M58" s="96"/>
       <c r="N58" s="97"/>
-      <c r="O58" s="140"/>
-      <c r="P58" s="145"/>
+      <c r="O58" s="139"/>
+      <c r="P58" s="144"/>
       <c r="Q58" s="93"/>
       <c r="R58" s="94"/>
       <c r="S58" s="94"/>
-      <c r="T58" s="145"/>
+      <c r="T58" s="144"/>
       <c r="U58" s="93"/>
       <c r="V58" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A59" s="143"/>
+      <c r="A59" s="142"/>
       <c r="B59" s="107"/>
       <c r="C59" s="107"/>
       <c r="D59" s="108"/>
@@ -5250,19 +5375,19 @@
       <c r="L59" s="77"/>
       <c r="M59" s="85"/>
       <c r="N59" s="98"/>
-      <c r="O59" s="141"/>
-      <c r="P59" s="146"/>
+      <c r="O59" s="140"/>
+      <c r="P59" s="145"/>
       <c r="Q59" s="93"/>
       <c r="R59" s="72"/>
       <c r="S59" s="72"/>
-      <c r="T59" s="147"/>
+      <c r="T59" s="146"/>
       <c r="U59" s="93"/>
       <c r="V59" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A60" s="143"/>
+      <c r="A60" s="142"/>
       <c r="B60" s="107"/>
       <c r="C60" s="107"/>
       <c r="D60" s="108"/>
@@ -5276,19 +5401,19 @@
       <c r="L60" s="77"/>
       <c r="M60" s="85"/>
       <c r="N60" s="97"/>
-      <c r="O60" s="140"/>
-      <c r="P60" s="146"/>
+      <c r="O60" s="139"/>
+      <c r="P60" s="145"/>
       <c r="Q60" s="93"/>
       <c r="R60" s="72"/>
       <c r="S60" s="72"/>
-      <c r="T60" s="147"/>
+      <c r="T60" s="146"/>
       <c r="U60" s="93"/>
       <c r="V60" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A61" s="143"/>
+      <c r="A61" s="142"/>
       <c r="B61" s="107"/>
       <c r="C61" s="107"/>
       <c r="D61" s="108"/>
@@ -5302,19 +5427,19 @@
       <c r="L61" s="90"/>
       <c r="M61" s="91"/>
       <c r="N61" s="92"/>
-      <c r="O61" s="141"/>
-      <c r="P61" s="145"/>
+      <c r="O61" s="140"/>
+      <c r="P61" s="144"/>
       <c r="Q61" s="93"/>
       <c r="R61" s="94"/>
       <c r="S61" s="94"/>
-      <c r="T61" s="145"/>
+      <c r="T61" s="144"/>
       <c r="U61" s="93"/>
       <c r="V61" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A62" s="143"/>
+      <c r="A62" s="142"/>
       <c r="B62" s="107"/>
       <c r="C62" s="107"/>
       <c r="D62" s="108"/>
@@ -5328,19 +5453,19 @@
       <c r="L62" s="90"/>
       <c r="M62" s="96"/>
       <c r="N62" s="97"/>
-      <c r="O62" s="140"/>
-      <c r="P62" s="145"/>
+      <c r="O62" s="139"/>
+      <c r="P62" s="144"/>
       <c r="Q62" s="93"/>
       <c r="R62" s="94"/>
       <c r="S62" s="94"/>
-      <c r="T62" s="145"/>
+      <c r="T62" s="144"/>
       <c r="U62" s="93"/>
       <c r="V62" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A63" s="143"/>
+      <c r="A63" s="142"/>
       <c r="B63" s="107"/>
       <c r="C63" s="107"/>
       <c r="D63" s="108"/>
@@ -5354,19 +5479,19 @@
       <c r="L63" s="90"/>
       <c r="M63" s="96"/>
       <c r="N63" s="97"/>
-      <c r="O63" s="140"/>
-      <c r="P63" s="145"/>
+      <c r="O63" s="139"/>
+      <c r="P63" s="144"/>
       <c r="Q63" s="93"/>
       <c r="R63" s="94"/>
       <c r="S63" s="94"/>
-      <c r="T63" s="145"/>
+      <c r="T63" s="144"/>
       <c r="U63" s="93"/>
       <c r="V63" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A64" s="143"/>
+      <c r="A64" s="142"/>
       <c r="B64" s="107"/>
       <c r="C64" s="107"/>
       <c r="D64" s="108"/>
@@ -5380,19 +5505,19 @@
       <c r="L64" s="90"/>
       <c r="M64" s="96"/>
       <c r="N64" s="98"/>
-      <c r="O64" s="141"/>
-      <c r="P64" s="145"/>
+      <c r="O64" s="140"/>
+      <c r="P64" s="144"/>
       <c r="Q64" s="93"/>
       <c r="R64" s="94"/>
       <c r="S64" s="94"/>
-      <c r="T64" s="145"/>
+      <c r="T64" s="144"/>
       <c r="U64" s="93"/>
       <c r="V64" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A65" s="143"/>
+      <c r="A65" s="142"/>
       <c r="B65" s="107"/>
       <c r="C65" s="107"/>
       <c r="D65" s="108"/>
@@ -5406,19 +5531,19 @@
       <c r="L65" s="90"/>
       <c r="M65" s="96"/>
       <c r="N65" s="97"/>
-      <c r="O65" s="140"/>
-      <c r="P65" s="145"/>
+      <c r="O65" s="139"/>
+      <c r="P65" s="144"/>
       <c r="Q65" s="93"/>
       <c r="R65" s="94"/>
       <c r="S65" s="94"/>
-      <c r="T65" s="145"/>
+      <c r="T65" s="144"/>
       <c r="U65" s="93"/>
       <c r="V65" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A66" s="143"/>
+      <c r="A66" s="142"/>
       <c r="B66" s="107"/>
       <c r="C66" s="107"/>
       <c r="D66" s="108"/>
@@ -5432,19 +5557,19 @@
       <c r="L66" s="90"/>
       <c r="M66" s="96"/>
       <c r="N66" s="97"/>
-      <c r="O66" s="140"/>
-      <c r="P66" s="145"/>
+      <c r="O66" s="139"/>
+      <c r="P66" s="144"/>
       <c r="Q66" s="93"/>
       <c r="R66" s="94"/>
       <c r="S66" s="94"/>
-      <c r="T66" s="145"/>
+      <c r="T66" s="144"/>
       <c r="U66" s="93"/>
       <c r="V66" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A67" s="143"/>
+      <c r="A67" s="142"/>
       <c r="B67" s="107"/>
       <c r="C67" s="107"/>
       <c r="D67" s="108"/>
@@ -5458,19 +5583,19 @@
       <c r="L67" s="77"/>
       <c r="M67" s="85"/>
       <c r="N67" s="98"/>
-      <c r="O67" s="141"/>
-      <c r="P67" s="146"/>
+      <c r="O67" s="140"/>
+      <c r="P67" s="145"/>
       <c r="Q67" s="93"/>
       <c r="R67" s="72"/>
       <c r="S67" s="72"/>
-      <c r="T67" s="147"/>
+      <c r="T67" s="146"/>
       <c r="U67" s="93"/>
       <c r="V67" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:22" s="5" customFormat="1" ht="11" customHeight="1">
-      <c r="A68" s="143"/>
+      <c r="A68" s="142"/>
       <c r="B68" s="107"/>
       <c r="C68" s="107"/>
       <c r="D68" s="108"/>
@@ -5484,19 +5609,19 @@
       <c r="L68" s="77"/>
       <c r="M68" s="85"/>
       <c r="N68" s="97"/>
-      <c r="O68" s="140"/>
-      <c r="P68" s="146"/>
+      <c r="O68" s="139"/>
+      <c r="P68" s="145"/>
       <c r="Q68" s="93"/>
       <c r="R68" s="72"/>
       <c r="S68" s="72"/>
-      <c r="T68" s="147"/>
+      <c r="T68" s="146"/>
       <c r="U68" s="93"/>
       <c r="V68" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:22" s="4" customFormat="1" ht="11" customHeight="1">
-      <c r="A69" s="143"/>
+      <c r="A69" s="142"/>
       <c r="B69" s="107"/>
       <c r="C69" s="107"/>
       <c r="D69" s="108"/>
@@ -5510,19 +5635,19 @@
       <c r="L69" s="90"/>
       <c r="M69" s="91"/>
       <c r="N69" s="92"/>
-      <c r="O69" s="141"/>
-      <c r="P69" s="145"/>
+      <c r="O69" s="140"/>
+      <c r="P69" s="144"/>
       <c r="Q69" s="93"/>
       <c r="R69" s="94"/>
       <c r="S69" s="94"/>
-      <c r="T69" s="145"/>
+      <c r="T69" s="144"/>
       <c r="U69" s="93"/>
       <c r="V69" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="4" customFormat="1" ht="11" customHeight="1">
-      <c r="A70" s="143"/>
+      <c r="A70" s="142"/>
       <c r="B70" s="107"/>
       <c r="C70" s="107"/>
       <c r="D70" s="108"/>
@@ -5536,19 +5661,19 @@
       <c r="L70" s="90"/>
       <c r="M70" s="96"/>
       <c r="N70" s="97"/>
-      <c r="O70" s="140"/>
-      <c r="P70" s="145"/>
+      <c r="O70" s="139"/>
+      <c r="P70" s="144"/>
       <c r="Q70" s="93"/>
       <c r="R70" s="94"/>
       <c r="S70" s="94"/>
-      <c r="T70" s="145"/>
+      <c r="T70" s="144"/>
       <c r="U70" s="93"/>
       <c r="V70" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:22" s="4" customFormat="1" ht="11" customHeight="1">
-      <c r="A71" s="143"/>
+      <c r="A71" s="142"/>
       <c r="B71" s="107"/>
       <c r="C71" s="107"/>
       <c r="D71" s="108"/>
@@ -5562,19 +5687,19 @@
       <c r="L71" s="90"/>
       <c r="M71" s="96"/>
       <c r="N71" s="97"/>
-      <c r="O71" s="140"/>
-      <c r="P71" s="145"/>
+      <c r="O71" s="139"/>
+      <c r="P71" s="144"/>
       <c r="Q71" s="93"/>
       <c r="R71" s="94"/>
       <c r="S71" s="94"/>
-      <c r="T71" s="145"/>
+      <c r="T71" s="144"/>
       <c r="U71" s="93"/>
       <c r="V71" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:22" s="4" customFormat="1" ht="11" customHeight="1">
-      <c r="A72" s="143"/>
+      <c r="A72" s="142"/>
       <c r="B72" s="107"/>
       <c r="C72" s="107"/>
       <c r="D72" s="108"/>
@@ -5588,19 +5713,19 @@
       <c r="L72" s="90"/>
       <c r="M72" s="96"/>
       <c r="N72" s="98"/>
-      <c r="O72" s="141"/>
-      <c r="P72" s="145"/>
+      <c r="O72" s="140"/>
+      <c r="P72" s="144"/>
       <c r="Q72" s="93"/>
       <c r="R72" s="94"/>
       <c r="S72" s="94"/>
-      <c r="T72" s="145"/>
+      <c r="T72" s="144"/>
       <c r="U72" s="93"/>
       <c r="V72" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:22" s="4" customFormat="1" ht="11" customHeight="1">
-      <c r="A73" s="143"/>
+      <c r="A73" s="142"/>
       <c r="B73" s="107"/>
       <c r="C73" s="107"/>
       <c r="D73" s="108"/>
@@ -5614,19 +5739,19 @@
       <c r="L73" s="90"/>
       <c r="M73" s="96"/>
       <c r="N73" s="97"/>
-      <c r="O73" s="140"/>
-      <c r="P73" s="145"/>
+      <c r="O73" s="139"/>
+      <c r="P73" s="144"/>
       <c r="Q73" s="93"/>
       <c r="R73" s="94"/>
       <c r="S73" s="94"/>
-      <c r="T73" s="145"/>
+      <c r="T73" s="144"/>
       <c r="U73" s="93"/>
       <c r="V73" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:22" s="4" customFormat="1" ht="11" customHeight="1">
-      <c r="A74" s="143"/>
+      <c r="A74" s="142"/>
       <c r="B74" s="107"/>
       <c r="C74" s="107"/>
       <c r="D74" s="108"/>
@@ -5640,19 +5765,19 @@
       <c r="L74" s="90"/>
       <c r="M74" s="96"/>
       <c r="N74" s="97"/>
-      <c r="O74" s="140"/>
-      <c r="P74" s="145"/>
+      <c r="O74" s="139"/>
+      <c r="P74" s="144"/>
       <c r="Q74" s="93"/>
       <c r="R74" s="94"/>
       <c r="S74" s="94"/>
-      <c r="T74" s="145"/>
+      <c r="T74" s="144"/>
       <c r="U74" s="93"/>
       <c r="V74" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:22">
-      <c r="A75" s="143"/>
+      <c r="A75" s="142"/>
       <c r="B75" s="107"/>
       <c r="C75" s="107"/>
       <c r="D75" s="108"/>
@@ -5666,19 +5791,19 @@
       <c r="L75" s="77"/>
       <c r="M75" s="85"/>
       <c r="N75" s="98"/>
-      <c r="O75" s="141"/>
-      <c r="P75" s="146"/>
+      <c r="O75" s="140"/>
+      <c r="P75" s="145"/>
       <c r="Q75" s="93"/>
       <c r="R75" s="72"/>
       <c r="S75" s="72"/>
-      <c r="T75" s="147"/>
+      <c r="T75" s="146"/>
       <c r="U75" s="93"/>
       <c r="V75" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:22">
-      <c r="A76" s="143"/>
+      <c r="A76" s="142"/>
       <c r="B76" s="107"/>
       <c r="C76" s="107"/>
       <c r="D76" s="108"/>
@@ -5692,19 +5817,19 @@
       <c r="L76" s="77"/>
       <c r="M76" s="85"/>
       <c r="N76" s="97"/>
-      <c r="O76" s="140"/>
-      <c r="P76" s="146"/>
+      <c r="O76" s="139"/>
+      <c r="P76" s="145"/>
       <c r="Q76" s="93"/>
       <c r="R76" s="72"/>
       <c r="S76" s="72"/>
-      <c r="T76" s="147"/>
+      <c r="T76" s="146"/>
       <c r="U76" s="93"/>
       <c r="V76" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:22">
-      <c r="A77" s="143"/>
+      <c r="A77" s="142"/>
       <c r="B77" s="107"/>
       <c r="C77" s="107"/>
       <c r="D77" s="108"/>
@@ -5718,19 +5843,19 @@
       <c r="L77" s="90"/>
       <c r="M77" s="91"/>
       <c r="N77" s="92"/>
-      <c r="O77" s="141"/>
-      <c r="P77" s="145"/>
+      <c r="O77" s="140"/>
+      <c r="P77" s="144"/>
       <c r="Q77" s="93"/>
       <c r="R77" s="94"/>
       <c r="S77" s="94"/>
-      <c r="T77" s="145"/>
+      <c r="T77" s="144"/>
       <c r="U77" s="93"/>
       <c r="V77" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:22">
-      <c r="A78" s="143"/>
+      <c r="A78" s="142"/>
       <c r="B78" s="107"/>
       <c r="C78" s="107"/>
       <c r="D78" s="108"/>
@@ -5744,19 +5869,19 @@
       <c r="L78" s="90"/>
       <c r="M78" s="96"/>
       <c r="N78" s="97"/>
-      <c r="O78" s="140"/>
-      <c r="P78" s="145"/>
+      <c r="O78" s="139"/>
+      <c r="P78" s="144"/>
       <c r="Q78" s="93"/>
       <c r="R78" s="94"/>
       <c r="S78" s="94"/>
-      <c r="T78" s="145"/>
+      <c r="T78" s="144"/>
       <c r="U78" s="93"/>
       <c r="V78" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:22">
-      <c r="A79" s="143"/>
+      <c r="A79" s="142"/>
       <c r="B79" s="107"/>
       <c r="C79" s="107"/>
       <c r="D79" s="108"/>
@@ -5770,19 +5895,19 @@
       <c r="L79" s="90"/>
       <c r="M79" s="96"/>
       <c r="N79" s="97"/>
-      <c r="O79" s="140"/>
-      <c r="P79" s="145"/>
+      <c r="O79" s="139"/>
+      <c r="P79" s="144"/>
       <c r="Q79" s="93"/>
       <c r="R79" s="94"/>
       <c r="S79" s="94"/>
-      <c r="T79" s="145"/>
+      <c r="T79" s="144"/>
       <c r="U79" s="93"/>
       <c r="V79" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:22">
-      <c r="A80" s="143"/>
+      <c r="A80" s="142"/>
       <c r="B80" s="107"/>
       <c r="C80" s="107"/>
       <c r="D80" s="108"/>
@@ -5796,19 +5921,19 @@
       <c r="L80" s="90"/>
       <c r="M80" s="96"/>
       <c r="N80" s="98"/>
-      <c r="O80" s="141"/>
-      <c r="P80" s="145"/>
+      <c r="O80" s="140"/>
+      <c r="P80" s="144"/>
       <c r="Q80" s="93"/>
       <c r="R80" s="94"/>
       <c r="S80" s="94"/>
-      <c r="T80" s="145"/>
+      <c r="T80" s="144"/>
       <c r="U80" s="93"/>
       <c r="V80" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:22">
-      <c r="A81" s="143"/>
+      <c r="A81" s="142"/>
       <c r="B81" s="107"/>
       <c r="C81" s="107"/>
       <c r="D81" s="108"/>
@@ -5822,19 +5947,19 @@
       <c r="L81" s="90"/>
       <c r="M81" s="96"/>
       <c r="N81" s="97"/>
-      <c r="O81" s="140"/>
-      <c r="P81" s="145"/>
+      <c r="O81" s="139"/>
+      <c r="P81" s="144"/>
       <c r="Q81" s="93"/>
       <c r="R81" s="94"/>
       <c r="S81" s="94"/>
-      <c r="T81" s="145"/>
+      <c r="T81" s="144"/>
       <c r="U81" s="93"/>
       <c r="V81" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:22">
-      <c r="A82" s="143"/>
+      <c r="A82" s="142"/>
       <c r="B82" s="107"/>
       <c r="C82" s="107"/>
       <c r="D82" s="108"/>
@@ -5848,19 +5973,19 @@
       <c r="L82" s="90"/>
       <c r="M82" s="96"/>
       <c r="N82" s="97"/>
-      <c r="O82" s="140"/>
-      <c r="P82" s="145"/>
+      <c r="O82" s="139"/>
+      <c r="P82" s="144"/>
       <c r="Q82" s="93"/>
       <c r="R82" s="94"/>
       <c r="S82" s="94"/>
-      <c r="T82" s="145"/>
+      <c r="T82" s="144"/>
       <c r="U82" s="93"/>
       <c r="V82" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:22">
-      <c r="A83" s="143"/>
+      <c r="A83" s="142"/>
       <c r="B83" s="107"/>
       <c r="C83" s="107"/>
       <c r="D83" s="108"/>
@@ -5874,19 +5999,19 @@
       <c r="L83" s="77"/>
       <c r="M83" s="85"/>
       <c r="N83" s="98"/>
-      <c r="O83" s="141"/>
-      <c r="P83" s="146"/>
+      <c r="O83" s="140"/>
+      <c r="P83" s="145"/>
       <c r="Q83" s="93"/>
       <c r="R83" s="72"/>
       <c r="S83" s="72"/>
-      <c r="T83" s="147"/>
+      <c r="T83" s="146"/>
       <c r="U83" s="93"/>
       <c r="V83" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:22">
-      <c r="A84" s="143"/>
+      <c r="A84" s="142"/>
       <c r="B84" s="107"/>
       <c r="C84" s="107"/>
       <c r="D84" s="108"/>
@@ -5900,19 +6025,19 @@
       <c r="L84" s="77"/>
       <c r="M84" s="85"/>
       <c r="N84" s="97"/>
-      <c r="O84" s="140"/>
-      <c r="P84" s="146"/>
+      <c r="O84" s="139"/>
+      <c r="P84" s="145"/>
       <c r="Q84" s="93"/>
       <c r="R84" s="72"/>
       <c r="S84" s="72"/>
-      <c r="T84" s="147"/>
+      <c r="T84" s="146"/>
       <c r="U84" s="93"/>
       <c r="V84" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:22">
-      <c r="A85" s="143"/>
+      <c r="A85" s="142"/>
       <c r="B85" s="107"/>
       <c r="C85" s="107"/>
       <c r="D85" s="108"/>
@@ -5926,19 +6051,19 @@
       <c r="L85" s="90"/>
       <c r="M85" s="91"/>
       <c r="N85" s="92"/>
-      <c r="O85" s="141"/>
-      <c r="P85" s="145"/>
+      <c r="O85" s="140"/>
+      <c r="P85" s="144"/>
       <c r="Q85" s="93"/>
       <c r="R85" s="94"/>
       <c r="S85" s="94"/>
-      <c r="T85" s="145"/>
+      <c r="T85" s="144"/>
       <c r="U85" s="93"/>
       <c r="V85" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:22">
-      <c r="A86" s="143"/>
+      <c r="A86" s="142"/>
       <c r="B86" s="107"/>
       <c r="C86" s="107"/>
       <c r="D86" s="108"/>
@@ -5952,19 +6077,19 @@
       <c r="L86" s="90"/>
       <c r="M86" s="96"/>
       <c r="N86" s="97"/>
-      <c r="O86" s="140"/>
-      <c r="P86" s="145"/>
+      <c r="O86" s="139"/>
+      <c r="P86" s="144"/>
       <c r="Q86" s="93"/>
       <c r="R86" s="94"/>
       <c r="S86" s="94"/>
-      <c r="T86" s="145"/>
+      <c r="T86" s="144"/>
       <c r="U86" s="93"/>
       <c r="V86" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:22">
-      <c r="A87" s="143"/>
+      <c r="A87" s="142"/>
       <c r="B87" s="107"/>
       <c r="C87" s="107"/>
       <c r="D87" s="108"/>
@@ -5978,19 +6103,19 @@
       <c r="L87" s="90"/>
       <c r="M87" s="96"/>
       <c r="N87" s="97"/>
-      <c r="O87" s="140"/>
-      <c r="P87" s="145"/>
+      <c r="O87" s="139"/>
+      <c r="P87" s="144"/>
       <c r="Q87" s="93"/>
       <c r="R87" s="94"/>
       <c r="S87" s="94"/>
-      <c r="T87" s="145"/>
+      <c r="T87" s="144"/>
       <c r="U87" s="93"/>
       <c r="V87" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:22">
-      <c r="A88" s="143"/>
+      <c r="A88" s="142"/>
       <c r="B88" s="107"/>
       <c r="C88" s="107"/>
       <c r="D88" s="108"/>
@@ -6004,19 +6129,19 @@
       <c r="L88" s="90"/>
       <c r="M88" s="96"/>
       <c r="N88" s="98"/>
-      <c r="O88" s="141"/>
-      <c r="P88" s="145"/>
+      <c r="O88" s="140"/>
+      <c r="P88" s="144"/>
       <c r="Q88" s="93"/>
       <c r="R88" s="94"/>
       <c r="S88" s="94"/>
-      <c r="T88" s="145"/>
+      <c r="T88" s="144"/>
       <c r="U88" s="93"/>
       <c r="V88" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:22">
-      <c r="A89" s="143"/>
+      <c r="A89" s="142"/>
       <c r="B89" s="107"/>
       <c r="C89" s="107"/>
       <c r="D89" s="108"/>
@@ -6030,19 +6155,19 @@
       <c r="L89" s="90"/>
       <c r="M89" s="96"/>
       <c r="N89" s="97"/>
-      <c r="O89" s="140"/>
-      <c r="P89" s="145"/>
+      <c r="O89" s="139"/>
+      <c r="P89" s="144"/>
       <c r="Q89" s="93"/>
       <c r="R89" s="94"/>
       <c r="S89" s="94"/>
-      <c r="T89" s="145"/>
+      <c r="T89" s="144"/>
       <c r="U89" s="93"/>
       <c r="V89" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:22">
-      <c r="A90" s="143"/>
+      <c r="A90" s="142"/>
       <c r="B90" s="107"/>
       <c r="C90" s="107"/>
       <c r="D90" s="108"/>
@@ -6056,19 +6181,19 @@
       <c r="L90" s="90"/>
       <c r="M90" s="96"/>
       <c r="N90" s="97"/>
-      <c r="O90" s="140"/>
-      <c r="P90" s="145"/>
+      <c r="O90" s="139"/>
+      <c r="P90" s="144"/>
       <c r="Q90" s="93"/>
       <c r="R90" s="94"/>
       <c r="S90" s="94"/>
-      <c r="T90" s="145"/>
+      <c r="T90" s="144"/>
       <c r="U90" s="93"/>
       <c r="V90" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:22">
-      <c r="A91" s="143"/>
+      <c r="A91" s="142"/>
       <c r="B91" s="107"/>
       <c r="C91" s="107"/>
       <c r="D91" s="108"/>
@@ -6082,19 +6207,19 @@
       <c r="L91" s="77"/>
       <c r="M91" s="85"/>
       <c r="N91" s="98"/>
-      <c r="O91" s="141"/>
-      <c r="P91" s="146"/>
+      <c r="O91" s="140"/>
+      <c r="P91" s="145"/>
       <c r="Q91" s="93"/>
       <c r="R91" s="72"/>
       <c r="S91" s="72"/>
-      <c r="T91" s="147"/>
+      <c r="T91" s="146"/>
       <c r="U91" s="93"/>
       <c r="V91" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:22">
-      <c r="A92" s="143"/>
+      <c r="A92" s="142"/>
       <c r="B92" s="107"/>
       <c r="C92" s="107"/>
       <c r="D92" s="108"/>
@@ -6108,19 +6233,19 @@
       <c r="L92" s="77"/>
       <c r="M92" s="85"/>
       <c r="N92" s="97"/>
-      <c r="O92" s="140"/>
-      <c r="P92" s="146"/>
+      <c r="O92" s="139"/>
+      <c r="P92" s="145"/>
       <c r="Q92" s="93"/>
       <c r="R92" s="72"/>
       <c r="S92" s="72"/>
-      <c r="T92" s="147"/>
+      <c r="T92" s="146"/>
       <c r="U92" s="93"/>
       <c r="V92" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:22">
-      <c r="A93" s="143"/>
+      <c r="A93" s="142"/>
       <c r="B93" s="107"/>
       <c r="C93" s="107"/>
       <c r="D93" s="108"/>
@@ -6134,19 +6259,19 @@
       <c r="L93" s="90"/>
       <c r="M93" s="91"/>
       <c r="N93" s="92"/>
-      <c r="O93" s="141"/>
-      <c r="P93" s="145"/>
+      <c r="O93" s="140"/>
+      <c r="P93" s="144"/>
       <c r="Q93" s="93"/>
       <c r="R93" s="94"/>
       <c r="S93" s="94"/>
-      <c r="T93" s="145"/>
+      <c r="T93" s="144"/>
       <c r="U93" s="93"/>
       <c r="V93" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:22">
-      <c r="A94" s="143"/>
+      <c r="A94" s="142"/>
       <c r="B94" s="107"/>
       <c r="C94" s="107"/>
       <c r="D94" s="108"/>
@@ -6160,19 +6285,19 @@
       <c r="L94" s="90"/>
       <c r="M94" s="96"/>
       <c r="N94" s="97"/>
-      <c r="O94" s="140"/>
-      <c r="P94" s="145"/>
+      <c r="O94" s="139"/>
+      <c r="P94" s="144"/>
       <c r="Q94" s="93"/>
       <c r="R94" s="94"/>
       <c r="S94" s="94"/>
-      <c r="T94" s="145"/>
+      <c r="T94" s="144"/>
       <c r="U94" s="93"/>
       <c r="V94" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:22">
-      <c r="A95" s="143"/>
+      <c r="A95" s="142"/>
       <c r="B95" s="107"/>
       <c r="C95" s="107"/>
       <c r="D95" s="108"/>
@@ -6186,19 +6311,19 @@
       <c r="L95" s="90"/>
       <c r="M95" s="96"/>
       <c r="N95" s="97"/>
-      <c r="O95" s="140"/>
-      <c r="P95" s="145"/>
+      <c r="O95" s="139"/>
+      <c r="P95" s="144"/>
       <c r="Q95" s="93"/>
       <c r="R95" s="94"/>
       <c r="S95" s="94"/>
-      <c r="T95" s="145"/>
+      <c r="T95" s="144"/>
       <c r="U95" s="93"/>
       <c r="V95" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:22">
-      <c r="A96" s="143"/>
+      <c r="A96" s="142"/>
       <c r="B96" s="107"/>
       <c r="C96" s="107"/>
       <c r="D96" s="108"/>
@@ -6212,19 +6337,19 @@
       <c r="L96" s="90"/>
       <c r="M96" s="96"/>
       <c r="N96" s="98"/>
-      <c r="O96" s="141"/>
-      <c r="P96" s="145"/>
+      <c r="O96" s="140"/>
+      <c r="P96" s="144"/>
       <c r="Q96" s="93"/>
       <c r="R96" s="94"/>
       <c r="S96" s="94"/>
-      <c r="T96" s="145"/>
+      <c r="T96" s="144"/>
       <c r="U96" s="93"/>
       <c r="V96" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:22">
-      <c r="A97" s="143"/>
+      <c r="A97" s="142"/>
       <c r="B97" s="107"/>
       <c r="C97" s="107"/>
       <c r="D97" s="108"/>
@@ -6238,19 +6363,19 @@
       <c r="L97" s="90"/>
       <c r="M97" s="96"/>
       <c r="N97" s="97"/>
-      <c r="O97" s="140"/>
-      <c r="P97" s="145"/>
+      <c r="O97" s="139"/>
+      <c r="P97" s="144"/>
       <c r="Q97" s="93"/>
       <c r="R97" s="94"/>
       <c r="S97" s="94"/>
-      <c r="T97" s="145"/>
+      <c r="T97" s="144"/>
       <c r="U97" s="93"/>
       <c r="V97" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:22">
-      <c r="A98" s="143"/>
+      <c r="A98" s="142"/>
       <c r="B98" s="107"/>
       <c r="C98" s="107"/>
       <c r="D98" s="108"/>
@@ -6264,19 +6389,19 @@
       <c r="L98" s="90"/>
       <c r="M98" s="96"/>
       <c r="N98" s="97"/>
-      <c r="O98" s="140"/>
-      <c r="P98" s="145"/>
+      <c r="O98" s="139"/>
+      <c r="P98" s="144"/>
       <c r="Q98" s="93"/>
       <c r="R98" s="94"/>
       <c r="S98" s="94"/>
-      <c r="T98" s="145"/>
+      <c r="T98" s="144"/>
       <c r="U98" s="93"/>
       <c r="V98" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:22">
-      <c r="A99" s="143"/>
+      <c r="A99" s="142"/>
       <c r="B99" s="107"/>
       <c r="C99" s="107"/>
       <c r="D99" s="108"/>
@@ -6290,19 +6415,19 @@
       <c r="L99" s="77"/>
       <c r="M99" s="85"/>
       <c r="N99" s="98"/>
-      <c r="O99" s="141"/>
-      <c r="P99" s="146"/>
+      <c r="O99" s="140"/>
+      <c r="P99" s="145"/>
       <c r="Q99" s="93"/>
       <c r="R99" s="72"/>
       <c r="S99" s="72"/>
-      <c r="T99" s="147"/>
+      <c r="T99" s="146"/>
       <c r="U99" s="93"/>
       <c r="V99" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:22">
-      <c r="A100" s="143"/>
+      <c r="A100" s="142"/>
       <c r="B100" s="107"/>
       <c r="C100" s="107"/>
       <c r="D100" s="108"/>
@@ -6316,19 +6441,19 @@
       <c r="L100" s="77"/>
       <c r="M100" s="85"/>
       <c r="N100" s="97"/>
-      <c r="O100" s="140"/>
-      <c r="P100" s="146"/>
+      <c r="O100" s="139"/>
+      <c r="P100" s="145"/>
       <c r="Q100" s="93"/>
       <c r="R100" s="72"/>
       <c r="S100" s="72"/>
-      <c r="T100" s="147"/>
+      <c r="T100" s="146"/>
       <c r="U100" s="93"/>
       <c r="V100" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:22">
-      <c r="A101" s="143"/>
+      <c r="A101" s="142"/>
       <c r="B101" s="107"/>
       <c r="C101" s="107"/>
       <c r="D101" s="108"/>
@@ -6342,19 +6467,19 @@
       <c r="L101" s="90"/>
       <c r="M101" s="91"/>
       <c r="N101" s="92"/>
-      <c r="O101" s="141"/>
-      <c r="P101" s="145"/>
+      <c r="O101" s="140"/>
+      <c r="P101" s="144"/>
       <c r="Q101" s="93"/>
       <c r="R101" s="94"/>
       <c r="S101" s="94"/>
-      <c r="T101" s="145"/>
+      <c r="T101" s="144"/>
       <c r="U101" s="93"/>
       <c r="V101" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:22">
-      <c r="A102" s="143"/>
+      <c r="A102" s="142"/>
       <c r="B102" s="107"/>
       <c r="C102" s="107"/>
       <c r="D102" s="108"/>
@@ -6368,19 +6493,19 @@
       <c r="L102" s="90"/>
       <c r="M102" s="96"/>
       <c r="N102" s="97"/>
-      <c r="O102" s="140"/>
-      <c r="P102" s="145"/>
+      <c r="O102" s="139"/>
+      <c r="P102" s="144"/>
       <c r="Q102" s="93"/>
       <c r="R102" s="94"/>
       <c r="S102" s="94"/>
-      <c r="T102" s="145"/>
+      <c r="T102" s="144"/>
       <c r="U102" s="93"/>
       <c r="V102" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:22">
-      <c r="A103" s="143"/>
+      <c r="A103" s="142"/>
       <c r="B103" s="107"/>
       <c r="C103" s="107"/>
       <c r="D103" s="108"/>
@@ -6394,19 +6519,19 @@
       <c r="L103" s="90"/>
       <c r="M103" s="96"/>
       <c r="N103" s="97"/>
-      <c r="O103" s="140"/>
-      <c r="P103" s="145"/>
+      <c r="O103" s="139"/>
+      <c r="P103" s="144"/>
       <c r="Q103" s="93"/>
       <c r="R103" s="94"/>
       <c r="S103" s="94"/>
-      <c r="T103" s="145"/>
+      <c r="T103" s="144"/>
       <c r="U103" s="93"/>
       <c r="V103" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:22">
-      <c r="A104" s="143"/>
+      <c r="A104" s="142"/>
       <c r="B104" s="107"/>
       <c r="C104" s="107"/>
       <c r="D104" s="108"/>
@@ -6420,19 +6545,19 @@
       <c r="L104" s="90"/>
       <c r="M104" s="96"/>
       <c r="N104" s="98"/>
-      <c r="O104" s="141"/>
-      <c r="P104" s="145"/>
+      <c r="O104" s="140"/>
+      <c r="P104" s="144"/>
       <c r="Q104" s="93"/>
       <c r="R104" s="94"/>
       <c r="S104" s="94"/>
-      <c r="T104" s="145"/>
+      <c r="T104" s="144"/>
       <c r="U104" s="93"/>
       <c r="V104" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:22">
-      <c r="A105" s="143"/>
+      <c r="A105" s="142"/>
       <c r="B105" s="107"/>
       <c r="C105" s="107"/>
       <c r="D105" s="108"/>
@@ -6446,19 +6571,19 @@
       <c r="L105" s="90"/>
       <c r="M105" s="96"/>
       <c r="N105" s="97"/>
-      <c r="O105" s="140"/>
-      <c r="P105" s="145"/>
+      <c r="O105" s="139"/>
+      <c r="P105" s="144"/>
       <c r="Q105" s="93"/>
       <c r="R105" s="94"/>
       <c r="S105" s="94"/>
-      <c r="T105" s="145"/>
+      <c r="T105" s="144"/>
       <c r="U105" s="93"/>
       <c r="V105" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:22">
-      <c r="A106" s="143"/>
+      <c r="A106" s="142"/>
       <c r="B106" s="107"/>
       <c r="C106" s="107"/>
       <c r="D106" s="108"/>
@@ -6472,19 +6597,19 @@
       <c r="L106" s="90"/>
       <c r="M106" s="96"/>
       <c r="N106" s="97"/>
-      <c r="O106" s="140"/>
-      <c r="P106" s="145"/>
+      <c r="O106" s="139"/>
+      <c r="P106" s="144"/>
       <c r="Q106" s="93"/>
       <c r="R106" s="94"/>
       <c r="S106" s="94"/>
-      <c r="T106" s="145"/>
+      <c r="T106" s="144"/>
       <c r="U106" s="93"/>
       <c r="V106" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:22">
-      <c r="A107" s="143"/>
+      <c r="A107" s="142"/>
       <c r="B107" s="107"/>
       <c r="C107" s="107"/>
       <c r="D107" s="108"/>
@@ -6498,19 +6623,19 @@
       <c r="L107" s="77"/>
       <c r="M107" s="85"/>
       <c r="N107" s="98"/>
-      <c r="O107" s="141"/>
-      <c r="P107" s="146"/>
+      <c r="O107" s="140"/>
+      <c r="P107" s="145"/>
       <c r="Q107" s="93"/>
       <c r="R107" s="72"/>
       <c r="S107" s="72"/>
-      <c r="T107" s="147"/>
+      <c r="T107" s="146"/>
       <c r="U107" s="93"/>
       <c r="V107" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:22">
-      <c r="A108" s="143"/>
+      <c r="A108" s="142"/>
       <c r="B108" s="107"/>
       <c r="C108" s="107"/>
       <c r="D108" s="108"/>
@@ -6524,19 +6649,19 @@
       <c r="L108" s="77"/>
       <c r="M108" s="85"/>
       <c r="N108" s="97"/>
-      <c r="O108" s="140"/>
-      <c r="P108" s="146"/>
+      <c r="O108" s="139"/>
+      <c r="P108" s="145"/>
       <c r="Q108" s="93"/>
       <c r="R108" s="72"/>
       <c r="S108" s="72"/>
-      <c r="T108" s="147"/>
+      <c r="T108" s="146"/>
       <c r="U108" s="93"/>
       <c r="V108" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:22">
-      <c r="A109" s="143"/>
+      <c r="A109" s="142"/>
       <c r="B109" s="107"/>
       <c r="C109" s="107"/>
       <c r="D109" s="108"/>
@@ -6550,19 +6675,19 @@
       <c r="L109" s="90"/>
       <c r="M109" s="91"/>
       <c r="N109" s="92"/>
-      <c r="O109" s="141"/>
-      <c r="P109" s="145"/>
+      <c r="O109" s="140"/>
+      <c r="P109" s="144"/>
       <c r="Q109" s="93"/>
       <c r="R109" s="94"/>
       <c r="S109" s="94"/>
-      <c r="T109" s="145"/>
+      <c r="T109" s="144"/>
       <c r="U109" s="93"/>
       <c r="V109" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:22">
-      <c r="A110" s="143"/>
+      <c r="A110" s="142"/>
       <c r="B110" s="107"/>
       <c r="C110" s="107"/>
       <c r="D110" s="108"/>
@@ -6576,19 +6701,19 @@
       <c r="L110" s="90"/>
       <c r="M110" s="96"/>
       <c r="N110" s="97"/>
-      <c r="O110" s="140"/>
-      <c r="P110" s="145"/>
+      <c r="O110" s="139"/>
+      <c r="P110" s="144"/>
       <c r="Q110" s="93"/>
       <c r="R110" s="94"/>
       <c r="S110" s="94"/>
-      <c r="T110" s="145"/>
+      <c r="T110" s="144"/>
       <c r="U110" s="93"/>
       <c r="V110" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:22">
-      <c r="A111" s="143"/>
+      <c r="A111" s="142"/>
       <c r="B111" s="107"/>
       <c r="C111" s="107"/>
       <c r="D111" s="108"/>
@@ -6602,19 +6727,19 @@
       <c r="L111" s="90"/>
       <c r="M111" s="96"/>
       <c r="N111" s="97"/>
-      <c r="O111" s="140"/>
-      <c r="P111" s="145"/>
+      <c r="O111" s="139"/>
+      <c r="P111" s="144"/>
       <c r="Q111" s="93"/>
       <c r="R111" s="94"/>
       <c r="S111" s="94"/>
-      <c r="T111" s="145"/>
+      <c r="T111" s="144"/>
       <c r="U111" s="93"/>
       <c r="V111" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:22">
-      <c r="A112" s="143"/>
+      <c r="A112" s="142"/>
       <c r="B112" s="107"/>
       <c r="C112" s="107"/>
       <c r="D112" s="108"/>
@@ -6628,19 +6753,19 @@
       <c r="L112" s="90"/>
       <c r="M112" s="96"/>
       <c r="N112" s="98"/>
-      <c r="O112" s="141"/>
-      <c r="P112" s="145"/>
+      <c r="O112" s="140"/>
+      <c r="P112" s="144"/>
       <c r="Q112" s="93"/>
       <c r="R112" s="94"/>
       <c r="S112" s="94"/>
-      <c r="T112" s="145"/>
+      <c r="T112" s="144"/>
       <c r="U112" s="93"/>
       <c r="V112" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:22">
-      <c r="A113" s="143"/>
+      <c r="A113" s="142"/>
       <c r="B113" s="107"/>
       <c r="C113" s="107"/>
       <c r="D113" s="108"/>
@@ -6654,19 +6779,19 @@
       <c r="L113" s="90"/>
       <c r="M113" s="96"/>
       <c r="N113" s="97"/>
-      <c r="O113" s="140"/>
-      <c r="P113" s="145"/>
+      <c r="O113" s="139"/>
+      <c r="P113" s="144"/>
       <c r="Q113" s="93"/>
       <c r="R113" s="94"/>
       <c r="S113" s="94"/>
-      <c r="T113" s="145"/>
+      <c r="T113" s="144"/>
       <c r="U113" s="93"/>
       <c r="V113" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:22">
-      <c r="A114" s="143"/>
+      <c r="A114" s="142"/>
       <c r="B114" s="107"/>
       <c r="C114" s="107"/>
       <c r="D114" s="108"/>
@@ -6680,19 +6805,19 @@
       <c r="L114" s="90"/>
       <c r="M114" s="96"/>
       <c r="N114" s="97"/>
-      <c r="O114" s="140"/>
-      <c r="P114" s="145"/>
+      <c r="O114" s="139"/>
+      <c r="P114" s="144"/>
       <c r="Q114" s="93"/>
       <c r="R114" s="94"/>
       <c r="S114" s="94"/>
-      <c r="T114" s="145"/>
+      <c r="T114" s="144"/>
       <c r="U114" s="93"/>
       <c r="V114" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:22">
-      <c r="A115" s="143"/>
+      <c r="A115" s="142"/>
       <c r="B115" s="107"/>
       <c r="C115" s="107"/>
       <c r="D115" s="108"/>
@@ -6706,19 +6831,19 @@
       <c r="L115" s="77"/>
       <c r="M115" s="85"/>
       <c r="N115" s="98"/>
-      <c r="O115" s="141"/>
-      <c r="P115" s="146"/>
+      <c r="O115" s="140"/>
+      <c r="P115" s="145"/>
       <c r="Q115" s="93"/>
       <c r="R115" s="72"/>
       <c r="S115" s="72"/>
-      <c r="T115" s="147"/>
+      <c r="T115" s="146"/>
       <c r="U115" s="93"/>
       <c r="V115" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:22">
-      <c r="A116" s="143"/>
+      <c r="A116" s="142"/>
       <c r="B116" s="107"/>
       <c r="C116" s="107"/>
       <c r="D116" s="108"/>
@@ -6732,19 +6857,19 @@
       <c r="L116" s="77"/>
       <c r="M116" s="85"/>
       <c r="N116" s="97"/>
-      <c r="O116" s="140"/>
-      <c r="P116" s="146"/>
+      <c r="O116" s="139"/>
+      <c r="P116" s="145"/>
       <c r="Q116" s="93"/>
       <c r="R116" s="72"/>
       <c r="S116" s="72"/>
-      <c r="T116" s="147"/>
+      <c r="T116" s="146"/>
       <c r="U116" s="93"/>
       <c r="V116" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:22">
-      <c r="A117" s="143"/>
+      <c r="A117" s="142"/>
       <c r="B117" s="107"/>
       <c r="C117" s="107"/>
       <c r="D117" s="108"/>
@@ -6758,19 +6883,19 @@
       <c r="L117" s="90"/>
       <c r="M117" s="91"/>
       <c r="N117" s="92"/>
-      <c r="O117" s="141"/>
-      <c r="P117" s="145"/>
+      <c r="O117" s="140"/>
+      <c r="P117" s="144"/>
       <c r="Q117" s="93"/>
       <c r="R117" s="94"/>
       <c r="S117" s="94"/>
-      <c r="T117" s="145"/>
+      <c r="T117" s="144"/>
       <c r="U117" s="93"/>
       <c r="V117" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:22">
-      <c r="A118" s="143"/>
+      <c r="A118" s="142"/>
       <c r="B118" s="107"/>
       <c r="C118" s="107"/>
       <c r="D118" s="108"/>
@@ -6784,19 +6909,19 @@
       <c r="L118" s="90"/>
       <c r="M118" s="96"/>
       <c r="N118" s="97"/>
-      <c r="O118" s="140"/>
-      <c r="P118" s="145"/>
+      <c r="O118" s="139"/>
+      <c r="P118" s="144"/>
       <c r="Q118" s="93"/>
       <c r="R118" s="94"/>
       <c r="S118" s="94"/>
-      <c r="T118" s="145"/>
+      <c r="T118" s="144"/>
       <c r="U118" s="93"/>
       <c r="V118" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:22">
-      <c r="A119" s="143"/>
+      <c r="A119" s="142"/>
       <c r="B119" s="107"/>
       <c r="C119" s="107"/>
       <c r="D119" s="108"/>
@@ -6810,19 +6935,19 @@
       <c r="L119" s="90"/>
       <c r="M119" s="96"/>
       <c r="N119" s="97"/>
-      <c r="O119" s="140"/>
-      <c r="P119" s="145"/>
+      <c r="O119" s="139"/>
+      <c r="P119" s="144"/>
       <c r="Q119" s="93"/>
       <c r="R119" s="94"/>
       <c r="S119" s="94"/>
-      <c r="T119" s="145"/>
+      <c r="T119" s="144"/>
       <c r="U119" s="93"/>
       <c r="V119" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:22">
-      <c r="A120" s="143"/>
+      <c r="A120" s="142"/>
       <c r="B120" s="107"/>
       <c r="C120" s="107"/>
       <c r="D120" s="108"/>
@@ -6836,19 +6961,19 @@
       <c r="L120" s="90"/>
       <c r="M120" s="96"/>
       <c r="N120" s="98"/>
-      <c r="O120" s="141"/>
-      <c r="P120" s="145"/>
+      <c r="O120" s="140"/>
+      <c r="P120" s="144"/>
       <c r="Q120" s="93"/>
       <c r="R120" s="94"/>
       <c r="S120" s="94"/>
-      <c r="T120" s="145"/>
+      <c r="T120" s="144"/>
       <c r="U120" s="93"/>
       <c r="V120" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:22">
-      <c r="A121" s="143"/>
+      <c r="A121" s="142"/>
       <c r="B121" s="107"/>
       <c r="C121" s="107"/>
       <c r="D121" s="108"/>
@@ -6862,19 +6987,19 @@
       <c r="L121" s="90"/>
       <c r="M121" s="96"/>
       <c r="N121" s="97"/>
-      <c r="O121" s="140"/>
-      <c r="P121" s="145"/>
+      <c r="O121" s="139"/>
+      <c r="P121" s="144"/>
       <c r="Q121" s="93"/>
       <c r="R121" s="94"/>
       <c r="S121" s="94"/>
-      <c r="T121" s="145"/>
+      <c r="T121" s="144"/>
       <c r="U121" s="93"/>
       <c r="V121" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:22">
-      <c r="A122" s="143"/>
+      <c r="A122" s="142"/>
       <c r="B122" s="107"/>
       <c r="C122" s="107"/>
       <c r="D122" s="108"/>
@@ -6888,19 +7013,19 @@
       <c r="L122" s="90"/>
       <c r="M122" s="96"/>
       <c r="N122" s="97"/>
-      <c r="O122" s="140"/>
-      <c r="P122" s="145"/>
+      <c r="O122" s="139"/>
+      <c r="P122" s="144"/>
       <c r="Q122" s="93"/>
       <c r="R122" s="94"/>
       <c r="S122" s="94"/>
-      <c r="T122" s="145"/>
+      <c r="T122" s="144"/>
       <c r="U122" s="93"/>
       <c r="V122" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:22">
-      <c r="A123" s="143"/>
+      <c r="A123" s="142"/>
       <c r="B123" s="107"/>
       <c r="C123" s="107"/>
       <c r="D123" s="108"/>
@@ -6914,19 +7039,19 @@
       <c r="L123" s="77"/>
       <c r="M123" s="85"/>
       <c r="N123" s="98"/>
-      <c r="O123" s="141"/>
-      <c r="P123" s="146"/>
+      <c r="O123" s="140"/>
+      <c r="P123" s="145"/>
       <c r="Q123" s="93"/>
       <c r="R123" s="72"/>
       <c r="S123" s="72"/>
-      <c r="T123" s="147"/>
+      <c r="T123" s="146"/>
       <c r="U123" s="93"/>
       <c r="V123" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:22">
-      <c r="A124" s="143"/>
+      <c r="A124" s="142"/>
       <c r="B124" s="107"/>
       <c r="C124" s="107"/>
       <c r="D124" s="108"/>
@@ -6940,19 +7065,19 @@
       <c r="L124" s="77"/>
       <c r="M124" s="85"/>
       <c r="N124" s="97"/>
-      <c r="O124" s="140"/>
-      <c r="P124" s="146"/>
+      <c r="O124" s="139"/>
+      <c r="P124" s="145"/>
       <c r="Q124" s="93"/>
       <c r="R124" s="72"/>
       <c r="S124" s="72"/>
-      <c r="T124" s="147"/>
+      <c r="T124" s="146"/>
       <c r="U124" s="93"/>
       <c r="V124" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:22">
-      <c r="A125" s="143"/>
+      <c r="A125" s="142"/>
       <c r="B125" s="107"/>
       <c r="C125" s="107"/>
       <c r="D125" s="108"/>
@@ -6966,19 +7091,19 @@
       <c r="L125" s="90"/>
       <c r="M125" s="91"/>
       <c r="N125" s="92"/>
-      <c r="O125" s="141"/>
-      <c r="P125" s="145"/>
+      <c r="O125" s="140"/>
+      <c r="P125" s="144"/>
       <c r="Q125" s="93"/>
       <c r="R125" s="94"/>
       <c r="S125" s="94"/>
-      <c r="T125" s="145"/>
+      <c r="T125" s="144"/>
       <c r="U125" s="93"/>
       <c r="V125" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:22">
-      <c r="A126" s="143"/>
+      <c r="A126" s="142"/>
       <c r="B126" s="107"/>
       <c r="C126" s="107"/>
       <c r="D126" s="108"/>
@@ -6992,19 +7117,19 @@
       <c r="L126" s="90"/>
       <c r="M126" s="96"/>
       <c r="N126" s="97"/>
-      <c r="O126" s="140"/>
-      <c r="P126" s="145"/>
+      <c r="O126" s="139"/>
+      <c r="P126" s="144"/>
       <c r="Q126" s="93"/>
       <c r="R126" s="94"/>
       <c r="S126" s="94"/>
-      <c r="T126" s="145"/>
+      <c r="T126" s="144"/>
       <c r="U126" s="93"/>
       <c r="V126" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:22">
-      <c r="A127" s="143"/>
+      <c r="A127" s="142"/>
       <c r="B127" s="107"/>
       <c r="C127" s="107"/>
       <c r="D127" s="108"/>
@@ -7018,19 +7143,19 @@
       <c r="L127" s="90"/>
       <c r="M127" s="96"/>
       <c r="N127" s="97"/>
-      <c r="O127" s="140"/>
-      <c r="P127" s="145"/>
+      <c r="O127" s="139"/>
+      <c r="P127" s="144"/>
       <c r="Q127" s="93"/>
       <c r="R127" s="94"/>
       <c r="S127" s="94"/>
-      <c r="T127" s="145"/>
+      <c r="T127" s="144"/>
       <c r="U127" s="93"/>
       <c r="V127" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:22">
-      <c r="A128" s="143"/>
+      <c r="A128" s="142"/>
       <c r="B128" s="107"/>
       <c r="C128" s="107"/>
       <c r="D128" s="108"/>
@@ -7044,19 +7169,19 @@
       <c r="L128" s="90"/>
       <c r="M128" s="96"/>
       <c r="N128" s="98"/>
-      <c r="O128" s="141"/>
-      <c r="P128" s="145"/>
+      <c r="O128" s="140"/>
+      <c r="P128" s="144"/>
       <c r="Q128" s="93"/>
       <c r="R128" s="94"/>
       <c r="S128" s="94"/>
-      <c r="T128" s="145"/>
+      <c r="T128" s="144"/>
       <c r="U128" s="93"/>
       <c r="V128" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:22">
-      <c r="A129" s="143"/>
+      <c r="A129" s="142"/>
       <c r="B129" s="107"/>
       <c r="C129" s="107"/>
       <c r="D129" s="108"/>
@@ -7070,19 +7195,19 @@
       <c r="L129" s="90"/>
       <c r="M129" s="96"/>
       <c r="N129" s="97"/>
-      <c r="O129" s="140"/>
-      <c r="P129" s="145"/>
+      <c r="O129" s="139"/>
+      <c r="P129" s="144"/>
       <c r="Q129" s="93"/>
       <c r="R129" s="94"/>
       <c r="S129" s="94"/>
-      <c r="T129" s="145"/>
+      <c r="T129" s="144"/>
       <c r="U129" s="93"/>
       <c r="V129" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:22">
-      <c r="A130" s="143"/>
+      <c r="A130" s="142"/>
       <c r="B130" s="107"/>
       <c r="C130" s="107"/>
       <c r="D130" s="108"/>
@@ -7096,19 +7221,19 @@
       <c r="L130" s="90"/>
       <c r="M130" s="96"/>
       <c r="N130" s="97"/>
-      <c r="O130" s="140"/>
-      <c r="P130" s="145"/>
+      <c r="O130" s="139"/>
+      <c r="P130" s="144"/>
       <c r="Q130" s="93"/>
       <c r="R130" s="94"/>
       <c r="S130" s="94"/>
-      <c r="T130" s="145"/>
+      <c r="T130" s="144"/>
       <c r="U130" s="93"/>
       <c r="V130" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:22">
-      <c r="A131" s="143"/>
+      <c r="A131" s="142"/>
       <c r="B131" s="107"/>
       <c r="C131" s="107"/>
       <c r="D131" s="108"/>
@@ -7122,19 +7247,19 @@
       <c r="L131" s="77"/>
       <c r="M131" s="85"/>
       <c r="N131" s="98"/>
-      <c r="O131" s="141"/>
-      <c r="P131" s="146"/>
+      <c r="O131" s="140"/>
+      <c r="P131" s="145"/>
       <c r="Q131" s="93"/>
       <c r="R131" s="72"/>
       <c r="S131" s="72"/>
-      <c r="T131" s="147"/>
+      <c r="T131" s="146"/>
       <c r="U131" s="93"/>
       <c r="V131" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:22">
-      <c r="A132" s="143"/>
+      <c r="A132" s="142"/>
       <c r="B132" s="107"/>
       <c r="C132" s="107"/>
       <c r="D132" s="108"/>
@@ -7148,19 +7273,19 @@
       <c r="L132" s="77"/>
       <c r="M132" s="85"/>
       <c r="N132" s="97"/>
-      <c r="O132" s="140"/>
-      <c r="P132" s="146"/>
+      <c r="O132" s="139"/>
+      <c r="P132" s="145"/>
       <c r="Q132" s="93"/>
       <c r="R132" s="72"/>
       <c r="S132" s="72"/>
-      <c r="T132" s="147"/>
+      <c r="T132" s="146"/>
       <c r="U132" s="93"/>
       <c r="V132" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:22">
-      <c r="A133" s="143"/>
+      <c r="A133" s="142"/>
       <c r="B133" s="107"/>
       <c r="C133" s="107"/>
       <c r="D133" s="108"/>
@@ -7174,19 +7299,19 @@
       <c r="L133" s="90"/>
       <c r="M133" s="91"/>
       <c r="N133" s="92"/>
-      <c r="O133" s="141"/>
-      <c r="P133" s="145"/>
+      <c r="O133" s="140"/>
+      <c r="P133" s="144"/>
       <c r="Q133" s="93"/>
       <c r="R133" s="94"/>
       <c r="S133" s="94"/>
-      <c r="T133" s="145"/>
+      <c r="T133" s="144"/>
       <c r="U133" s="93"/>
       <c r="V133" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:22">
-      <c r="A134" s="143"/>
+      <c r="A134" s="142"/>
       <c r="B134" s="107"/>
       <c r="C134" s="107"/>
       <c r="D134" s="108"/>
@@ -7200,19 +7325,19 @@
       <c r="L134" s="90"/>
       <c r="M134" s="96"/>
       <c r="N134" s="97"/>
-      <c r="O134" s="140"/>
-      <c r="P134" s="145"/>
+      <c r="O134" s="139"/>
+      <c r="P134" s="144"/>
       <c r="Q134" s="93"/>
       <c r="R134" s="94"/>
       <c r="S134" s="94"/>
-      <c r="T134" s="145"/>
+      <c r="T134" s="144"/>
       <c r="U134" s="93"/>
       <c r="V134" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:22">
-      <c r="A135" s="143"/>
+      <c r="A135" s="142"/>
       <c r="B135" s="107"/>
       <c r="C135" s="107"/>
       <c r="D135" s="108"/>
@@ -7226,19 +7351,19 @@
       <c r="L135" s="90"/>
       <c r="M135" s="96"/>
       <c r="N135" s="97"/>
-      <c r="O135" s="140"/>
-      <c r="P135" s="145"/>
+      <c r="O135" s="139"/>
+      <c r="P135" s="144"/>
       <c r="Q135" s="93"/>
       <c r="R135" s="94"/>
       <c r="S135" s="94"/>
-      <c r="T135" s="145"/>
+      <c r="T135" s="144"/>
       <c r="U135" s="93"/>
       <c r="V135" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:22">
-      <c r="A136" s="143"/>
+      <c r="A136" s="142"/>
       <c r="B136" s="107"/>
       <c r="C136" s="107"/>
       <c r="D136" s="108"/>
@@ -7252,19 +7377,19 @@
       <c r="L136" s="90"/>
       <c r="M136" s="96"/>
       <c r="N136" s="98"/>
-      <c r="O136" s="141"/>
-      <c r="P136" s="145"/>
+      <c r="O136" s="140"/>
+      <c r="P136" s="144"/>
       <c r="Q136" s="93"/>
       <c r="R136" s="94"/>
       <c r="S136" s="94"/>
-      <c r="T136" s="145"/>
+      <c r="T136" s="144"/>
       <c r="U136" s="93"/>
       <c r="V136" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:22">
-      <c r="A137" s="143"/>
+      <c r="A137" s="142"/>
       <c r="B137" s="107"/>
       <c r="C137" s="107"/>
       <c r="D137" s="108"/>
@@ -7278,19 +7403,19 @@
       <c r="L137" s="90"/>
       <c r="M137" s="96"/>
       <c r="N137" s="97"/>
-      <c r="O137" s="140"/>
-      <c r="P137" s="145"/>
+      <c r="O137" s="139"/>
+      <c r="P137" s="144"/>
       <c r="Q137" s="93"/>
       <c r="R137" s="94"/>
       <c r="S137" s="94"/>
-      <c r="T137" s="145"/>
+      <c r="T137" s="144"/>
       <c r="U137" s="93"/>
       <c r="V137" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:22">
-      <c r="A138" s="143"/>
+      <c r="A138" s="142"/>
       <c r="B138" s="107"/>
       <c r="C138" s="107"/>
       <c r="D138" s="108"/>
@@ -7304,19 +7429,19 @@
       <c r="L138" s="90"/>
       <c r="M138" s="96"/>
       <c r="N138" s="97"/>
-      <c r="O138" s="140"/>
-      <c r="P138" s="145"/>
+      <c r="O138" s="139"/>
+      <c r="P138" s="144"/>
       <c r="Q138" s="93"/>
       <c r="R138" s="94"/>
       <c r="S138" s="94"/>
-      <c r="T138" s="145"/>
+      <c r="T138" s="144"/>
       <c r="U138" s="93"/>
       <c r="V138" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:22">
-      <c r="A139" s="143"/>
+      <c r="A139" s="142"/>
       <c r="B139" s="107"/>
       <c r="C139" s="107"/>
       <c r="D139" s="108"/>
@@ -7330,19 +7455,19 @@
       <c r="L139" s="77"/>
       <c r="M139" s="85"/>
       <c r="N139" s="98"/>
-      <c r="O139" s="141"/>
-      <c r="P139" s="146"/>
+      <c r="O139" s="140"/>
+      <c r="P139" s="145"/>
       <c r="Q139" s="93"/>
       <c r="R139" s="72"/>
       <c r="S139" s="72"/>
-      <c r="T139" s="147"/>
+      <c r="T139" s="146"/>
       <c r="U139" s="93"/>
       <c r="V139" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:22">
-      <c r="A140" s="143"/>
+      <c r="A140" s="142"/>
       <c r="B140" s="107"/>
       <c r="C140" s="107"/>
       <c r="D140" s="108"/>
@@ -7356,19 +7481,19 @@
       <c r="L140" s="77"/>
       <c r="M140" s="85"/>
       <c r="N140" s="97"/>
-      <c r="O140" s="140"/>
-      <c r="P140" s="146"/>
+      <c r="O140" s="139"/>
+      <c r="P140" s="145"/>
       <c r="Q140" s="93"/>
       <c r="R140" s="72"/>
       <c r="S140" s="72"/>
-      <c r="T140" s="147"/>
+      <c r="T140" s="146"/>
       <c r="U140" s="93"/>
       <c r="V140" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:22">
-      <c r="A141" s="143"/>
+      <c r="A141" s="142"/>
       <c r="B141" s="107"/>
       <c r="C141" s="107"/>
       <c r="D141" s="108"/>
@@ -7382,19 +7507,19 @@
       <c r="L141" s="90"/>
       <c r="M141" s="91"/>
       <c r="N141" s="92"/>
-      <c r="O141" s="141"/>
-      <c r="P141" s="145"/>
+      <c r="O141" s="140"/>
+      <c r="P141" s="144"/>
       <c r="Q141" s="93"/>
       <c r="R141" s="94"/>
       <c r="S141" s="94"/>
-      <c r="T141" s="145"/>
+      <c r="T141" s="144"/>
       <c r="U141" s="93"/>
       <c r="V141" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:22">
-      <c r="A142" s="143"/>
+      <c r="A142" s="142"/>
       <c r="B142" s="107"/>
       <c r="C142" s="107"/>
       <c r="D142" s="108"/>
@@ -7408,19 +7533,19 @@
       <c r="L142" s="90"/>
       <c r="M142" s="96"/>
       <c r="N142" s="97"/>
-      <c r="O142" s="140"/>
-      <c r="P142" s="145"/>
+      <c r="O142" s="139"/>
+      <c r="P142" s="144"/>
       <c r="Q142" s="93"/>
       <c r="R142" s="94"/>
       <c r="S142" s="94"/>
-      <c r="T142" s="145"/>
+      <c r="T142" s="144"/>
       <c r="U142" s="93"/>
       <c r="V142" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:22">
-      <c r="A143" s="143"/>
+      <c r="A143" s="142"/>
       <c r="B143" s="107"/>
       <c r="C143" s="107"/>
       <c r="D143" s="108"/>
@@ -7434,19 +7559,19 @@
       <c r="L143" s="90"/>
       <c r="M143" s="96"/>
       <c r="N143" s="97"/>
-      <c r="O143" s="140"/>
-      <c r="P143" s="145"/>
+      <c r="O143" s="139"/>
+      <c r="P143" s="144"/>
       <c r="Q143" s="93"/>
       <c r="R143" s="94"/>
       <c r="S143" s="94"/>
-      <c r="T143" s="145"/>
+      <c r="T143" s="144"/>
       <c r="U143" s="93"/>
       <c r="V143" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:22">
-      <c r="A144" s="143"/>
+      <c r="A144" s="142"/>
       <c r="B144" s="107"/>
       <c r="C144" s="107"/>
       <c r="D144" s="108"/>
@@ -7460,19 +7585,19 @@
       <c r="L144" s="90"/>
       <c r="M144" s="96"/>
       <c r="N144" s="98"/>
-      <c r="O144" s="141"/>
-      <c r="P144" s="145"/>
+      <c r="O144" s="140"/>
+      <c r="P144" s="144"/>
       <c r="Q144" s="93"/>
       <c r="R144" s="94"/>
       <c r="S144" s="94"/>
-      <c r="T144" s="145"/>
+      <c r="T144" s="144"/>
       <c r="U144" s="93"/>
       <c r="V144" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:22">
-      <c r="A145" s="143"/>
+      <c r="A145" s="142"/>
       <c r="B145" s="107"/>
       <c r="C145" s="107"/>
       <c r="D145" s="108"/>
@@ -7486,19 +7611,19 @@
       <c r="L145" s="90"/>
       <c r="M145" s="96"/>
       <c r="N145" s="97"/>
-      <c r="O145" s="140"/>
-      <c r="P145" s="145"/>
+      <c r="O145" s="139"/>
+      <c r="P145" s="144"/>
       <c r="Q145" s="93"/>
       <c r="R145" s="94"/>
       <c r="S145" s="94"/>
-      <c r="T145" s="145"/>
+      <c r="T145" s="144"/>
       <c r="U145" s="93"/>
       <c r="V145" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:22">
-      <c r="A146" s="143"/>
+      <c r="A146" s="142"/>
       <c r="B146" s="107"/>
       <c r="C146" s="107"/>
       <c r="D146" s="108"/>
@@ -7512,19 +7637,19 @@
       <c r="L146" s="90"/>
       <c r="M146" s="96"/>
       <c r="N146" s="97"/>
-      <c r="O146" s="140"/>
-      <c r="P146" s="145"/>
+      <c r="O146" s="139"/>
+      <c r="P146" s="144"/>
       <c r="Q146" s="93"/>
       <c r="R146" s="94"/>
       <c r="S146" s="94"/>
-      <c r="T146" s="145"/>
+      <c r="T146" s="144"/>
       <c r="U146" s="93"/>
       <c r="V146" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:22">
-      <c r="A147" s="143"/>
+      <c r="A147" s="142"/>
       <c r="B147" s="107"/>
       <c r="C147" s="107"/>
       <c r="D147" s="108"/>
@@ -7538,19 +7663,19 @@
       <c r="L147" s="77"/>
       <c r="M147" s="85"/>
       <c r="N147" s="98"/>
-      <c r="O147" s="141"/>
-      <c r="P147" s="146"/>
+      <c r="O147" s="140"/>
+      <c r="P147" s="145"/>
       <c r="Q147" s="93"/>
       <c r="R147" s="72"/>
       <c r="S147" s="72"/>
-      <c r="T147" s="147"/>
+      <c r="T147" s="146"/>
       <c r="U147" s="93"/>
       <c r="V147" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:22">
-      <c r="A148" s="143"/>
+      <c r="A148" s="142"/>
       <c r="B148" s="107"/>
       <c r="C148" s="107"/>
       <c r="D148" s="108"/>
@@ -7564,19 +7689,19 @@
       <c r="L148" s="77"/>
       <c r="M148" s="85"/>
       <c r="N148" s="97"/>
-      <c r="O148" s="140"/>
-      <c r="P148" s="146"/>
+      <c r="O148" s="139"/>
+      <c r="P148" s="145"/>
       <c r="Q148" s="93"/>
       <c r="R148" s="72"/>
       <c r="S148" s="72"/>
-      <c r="T148" s="147"/>
+      <c r="T148" s="146"/>
       <c r="U148" s="93"/>
       <c r="V148" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:22">
-      <c r="A149" s="143"/>
+      <c r="A149" s="142"/>
       <c r="B149" s="107"/>
       <c r="C149" s="107"/>
       <c r="D149" s="108"/>
@@ -7590,19 +7715,19 @@
       <c r="L149" s="90"/>
       <c r="M149" s="91"/>
       <c r="N149" s="92"/>
-      <c r="O149" s="141"/>
-      <c r="P149" s="145"/>
+      <c r="O149" s="140"/>
+      <c r="P149" s="144"/>
       <c r="Q149" s="93"/>
       <c r="R149" s="94"/>
       <c r="S149" s="94"/>
-      <c r="T149" s="145"/>
+      <c r="T149" s="144"/>
       <c r="U149" s="93"/>
       <c r="V149" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:22">
-      <c r="A150" s="143"/>
+      <c r="A150" s="142"/>
       <c r="B150" s="107"/>
       <c r="C150" s="107"/>
       <c r="D150" s="108"/>
@@ -7616,12 +7741,12 @@
       <c r="L150" s="90"/>
       <c r="M150" s="96"/>
       <c r="N150" s="97"/>
-      <c r="O150" s="140"/>
-      <c r="P150" s="145"/>
+      <c r="O150" s="139"/>
+      <c r="P150" s="144"/>
       <c r="Q150" s="93"/>
       <c r="R150" s="94"/>
       <c r="S150" s="94"/>
-      <c r="T150" s="145"/>
+      <c r="T150" s="144"/>
       <c r="U150" s="93"/>
       <c r="V150" s="30" t="s">
         <v>17</v>
@@ -7635,7 +7760,6 @@
       <c r="C151" s="73"/>
     </row>
   </sheetData>
-  <sheetProtection password="83BD" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="R15:T15"/>
@@ -7746,289 +7870,289 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="88" style="121" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="121" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="121"/>
+    <col min="1" max="1" width="88" style="120" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="120" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="120"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14">
-      <c r="A1" s="119"/>
-      <c r="B1" s="119" t="s">
+      <c r="A1" s="118"/>
+      <c r="B1" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="C1" s="118" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="120"/>
+      <c r="D1" s="119"/>
       <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="17" hidden="1">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="122"/>
+      <c r="A2" s="119"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="121"/>
     </row>
     <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="123"/>
-      <c r="B3" s="123" t="s">
+      <c r="A3" s="122"/>
+      <c r="B3" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="119" t="s">
         <v>289</v>
       </c>
-      <c r="D3" s="124" t="s">
+      <c r="D3" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="125"/>
+      <c r="E3" s="124"/>
     </row>
     <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="123"/>
-      <c r="B4" s="123" t="s">
+      <c r="A4" s="122"/>
+      <c r="B4" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="124" t="s">
+      <c r="C4" s="119"/>
+      <c r="D4" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="126" t="s">
+      <c r="E4" s="125" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:5" hidden="1"/>
     <row r="6" spans="1:5" hidden="1"/>
     <row r="14" spans="1:5" ht="19">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="116" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="133" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26">
-      <c r="A16" s="128" t="s">
+      <c r="A16" s="127" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="16">
-      <c r="A18" s="127" t="s">
+      <c r="A18" s="126" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="26">
-      <c r="A19" s="128" t="s">
+      <c r="A19" s="127" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="65">
-      <c r="A20" s="128" t="s">
+      <c r="A20" s="127" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="39">
-      <c r="A21" s="128" t="s">
+      <c r="A21" s="127" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="16">
-      <c r="A23" s="127" t="s">
+      <c r="A23" s="126" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="129" t="s">
+      <c r="A24" s="128" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="39">
-      <c r="A25" s="130" t="s">
+      <c r="A25" s="129" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20" customHeight="1">
-      <c r="A26" s="131" t="s">
+      <c r="A26" s="130" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20" customHeight="1">
-      <c r="A27" s="131" t="s">
+      <c r="A27" s="130" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="26">
-      <c r="A28" s="131" t="s">
+      <c r="A28" s="130" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="26">
-      <c r="A29" s="131" t="s">
+      <c r="A29" s="130" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="26">
-      <c r="A30" s="131" t="s">
+      <c r="A30" s="130" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="65">
-      <c r="A31" s="130" t="s">
+      <c r="A31" s="129" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="26">
-      <c r="A32" s="131" t="s">
+      <c r="A32" s="130" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="27" customHeight="1">
-      <c r="A33" s="148" t="s">
+      <c r="A33" s="147" t="s">
         <v>285</v>
       </c>
-      <c r="C33" s="128"/>
-      <c r="E33" s="128"/>
+      <c r="C33" s="127"/>
+      <c r="E33" s="127"/>
     </row>
     <row r="34" spans="1:5" ht="26">
-      <c r="A34" s="131" t="s">
+      <c r="A34" s="130" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="26">
-      <c r="A35" s="130" t="s">
+      <c r="A35" s="129" t="s">
         <v>287</v>
       </c>
-      <c r="C35" s="128"/>
-      <c r="E35" s="128"/>
+      <c r="C35" s="127"/>
+      <c r="E35" s="127"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36"/>
-      <c r="C36" s="128"/>
-      <c r="E36" s="128"/>
+      <c r="C36" s="127"/>
+      <c r="E36" s="127"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="129" t="s">
+      <c r="A37" s="128" t="s">
         <v>272</v>
       </c>
-      <c r="E37" s="128"/>
+      <c r="E37" s="127"/>
     </row>
     <row r="38" spans="1:5" ht="26">
-      <c r="A38" s="130" t="s">
+      <c r="A38" s="129" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="24" customHeight="1">
-      <c r="A39" s="132" t="s">
+      <c r="A39" s="131" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="24" customHeight="1">
-      <c r="A40" s="132"/>
+      <c r="A40" s="131"/>
     </row>
     <row r="41" spans="1:5" ht="24" customHeight="1">
-      <c r="A41" s="129" t="s">
+      <c r="A41" s="128" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="24" customHeight="1">
-      <c r="A42" s="142" t="s">
+      <c r="A42" s="141" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="118"/>
+      <c r="A43" s="117"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="129" t="s">
+      <c r="A44" s="128" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="26">
-      <c r="A45" s="130" t="s">
+      <c r="A45" s="129" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="26">
-      <c r="A46" s="130" t="s">
+      <c r="A46" s="129" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="132" t="s">
+      <c r="A47" s="131" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="128"/>
+      <c r="A48" s="127"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="128"/>
+      <c r="A49" s="127"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="128"/>
+      <c r="A50" s="127"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="133"/>
+      <c r="A51" s="132"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="128"/>
+      <c r="A52" s="127"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="128"/>
+      <c r="A53" s="127"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="128"/>
+      <c r="A54" s="127"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="128"/>
+      <c r="A55" s="127"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="128"/>
+      <c r="A56" s="127"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="128"/>
+      <c r="A57" s="127"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="128"/>
+      <c r="A58" s="127"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="128"/>
+      <c r="A59" s="127"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="128"/>
+      <c r="A60" s="127"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="128"/>
+      <c r="A61" s="127"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="128"/>
+      <c r="A62" s="127"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="128"/>
+      <c r="A63" s="127"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="128"/>
+      <c r="A64" s="127"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="128"/>
+      <c r="A65" s="127"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="128"/>
+      <c r="A66" s="127"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="128"/>
+      <c r="A67" s="127"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="128"/>
+      <c r="A68" s="127"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="128"/>
+      <c r="A69" s="127"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="128"/>
+      <c r="A70" s="127"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="128"/>
+      <c r="A71" s="127"/>
     </row>
   </sheetData>
   <sheetProtection password="83BD" sheet="1" objects="1" scenarios="1"/>
@@ -8071,7 +8195,7 @@
       <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="136" t="s">
+      <c r="C1" s="135" t="s">
         <v>300</v>
       </c>
       <c r="D1" t="s">
@@ -8103,7 +8227,7 @@
       <c r="B2" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="135" t="s">
+      <c r="C2" s="134" t="s">
         <v>80</v>
       </c>
       <c r="D2" t="s">
@@ -8129,7 +8253,7 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="134" t="s">
         <v>201</v>
       </c>
       <c r="D3" t="s">
@@ -8152,7 +8276,7 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="134" t="s">
         <v>202</v>
       </c>
       <c r="D4" t="s">
@@ -8172,7 +8296,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="C5" s="135" t="s">
+      <c r="C5" s="134" t="s">
         <v>200</v>
       </c>
       <c r="D5" t="s">
@@ -8192,7 +8316,7 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="C6" s="135" t="s">
+      <c r="C6" s="134" t="s">
         <v>84</v>
       </c>
       <c r="D6" t="s">
@@ -8210,7 +8334,7 @@
       <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="C7" s="135" t="s">
+      <c r="C7" s="134" t="s">
         <v>203</v>
       </c>
       <c r="D7" t="s">
@@ -8226,7 +8350,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="C8" s="135" t="s">
+      <c r="C8" s="134" t="s">
         <v>199</v>
       </c>
       <c r="D8" t="s">

</xml_diff>

<commit_message>
save strain & strain_other in status-db
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1603.6.microbial.xlsx
+++ b/tests/fixtures/orderforms/1603.6.microbial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A63A28F6-84E2-DF44-AF48-9B3942D5A569}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C5F137-D9A5-8E49-A1D6-877C9B766283}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" tabRatio="593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="49600" windowHeight="26740" tabRatio="593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order form" sheetId="1" r:id="rId1"/>
@@ -2732,27 +2732,27 @@
     <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="305">
@@ -3547,7 +3547,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3591,7 +3591,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3619,7 +3619,7 @@
   <dimension ref="A1:V151"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -4009,39 +4009,39 @@
       <c r="U14" s="59"/>
       <c r="V14" s="57"/>
     </row>
-    <row r="15" spans="1:22" s="7" customFormat="1" ht="22">
-      <c r="A15" s="148" t="s">
+    <row r="15" spans="1:22" s="7" customFormat="1" ht="24">
+      <c r="A15" s="150" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="149"/>
-      <c r="D15" s="149"/>
-      <c r="E15" s="149"/>
-      <c r="F15" s="149"/>
-      <c r="G15" s="149"/>
-      <c r="H15" s="149"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="149"/>
-      <c r="K15" s="150"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="152"/>
       <c r="L15" s="74"/>
-      <c r="M15" s="152" t="s">
+      <c r="M15" s="154" t="s">
         <v>108</v>
       </c>
-      <c r="N15" s="153"/>
+      <c r="N15" s="155"/>
       <c r="O15" s="136"/>
       <c r="P15" s="83" t="s">
         <v>308</v>
       </c>
       <c r="Q15" s="60"/>
-      <c r="R15" s="148" t="s">
+      <c r="R15" s="150" t="s">
         <v>106</v>
       </c>
-      <c r="S15" s="149"/>
-      <c r="T15" s="151"/>
+      <c r="S15" s="151"/>
+      <c r="T15" s="153"/>
       <c r="U15" s="23"/>
       <c r="V15" s="23"/>
     </row>
-    <row r="16" spans="1:22" s="7" customFormat="1" ht="11" hidden="1">
+    <row r="16" spans="1:22" s="7" customFormat="1" ht="12" hidden="1">
       <c r="A16" s="61" t="s">
         <v>0</v>
       </c>
@@ -4067,7 +4067,7 @@
       <c r="U16" s="23"/>
       <c r="V16" s="23"/>
     </row>
-    <row r="17" spans="1:22" s="8" customFormat="1" ht="33" hidden="1">
+    <row r="17" spans="1:22" s="8" customFormat="1" ht="36" hidden="1">
       <c r="A17" s="20" t="s">
         <v>1</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="9" customFormat="1" ht="11" hidden="1">
+    <row r="18" spans="1:22" s="9" customFormat="1" ht="12" hidden="1">
       <c r="A18" s="61" t="s">
         <v>5</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="U18" s="25"/>
       <c r="V18" s="22"/>
     </row>
-    <row r="19" spans="1:22" s="11" customFormat="1" ht="33">
+    <row r="19" spans="1:22" s="11" customFormat="1" ht="36">
       <c r="A19" s="26" t="s">
         <v>86</v>
       </c>
@@ -4240,7 +4240,7 @@
       <c r="V20" s="27"/>
     </row>
     <row r="21" spans="1:22" s="115" customFormat="1" ht="13" customHeight="1">
-      <c r="A21" s="154" t="s">
+      <c r="A21" s="148" t="s">
         <v>335</v>
       </c>
       <c r="B21" s="107" t="s">
@@ -4271,10 +4271,10 @@
         <v>9</v>
       </c>
       <c r="K21" s="107" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="L21" s="111"/>
-      <c r="M21" s="154" t="s">
+      <c r="M21" s="148" t="s">
         <v>330</v>
       </c>
       <c r="N21" s="112" t="s">
@@ -4291,7 +4291,7 @@
       <c r="S21" s="114">
         <v>102</v>
       </c>
-      <c r="T21" s="154" t="s">
+      <c r="T21" s="148" t="s">
         <v>331</v>
       </c>
       <c r="U21" s="113"/>
@@ -4300,7 +4300,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A22" s="154" t="s">
+      <c r="A22" s="148" t="s">
         <v>336</v>
       </c>
       <c r="B22" s="107" t="s">
@@ -4348,7 +4348,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A23" s="154" t="s">
+      <c r="A23" s="148" t="s">
         <v>337</v>
       </c>
       <c r="B23" s="107" t="s">
@@ -4379,10 +4379,10 @@
         <v>9</v>
       </c>
       <c r="K23" s="107" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="L23" s="90"/>
-      <c r="M23" s="155" t="s">
+      <c r="M23" s="149" t="s">
         <v>330</v>
       </c>
       <c r="N23" s="97" t="s">
@@ -4400,7 +4400,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="148" t="s">
         <v>338</v>
       </c>
       <c r="B24" s="107" t="s">
@@ -4431,7 +4431,7 @@
         <v>104</v>
       </c>
       <c r="K24" s="107" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="L24" s="90"/>
       <c r="M24" s="96"/>
@@ -4450,7 +4450,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" s="95" customFormat="1" ht="13" customHeight="1">
-      <c r="A25" s="154" t="s">
+      <c r="A25" s="148" t="s">
         <v>339</v>
       </c>
       <c r="B25" s="107" t="s">
@@ -4481,7 +4481,7 @@
         <v>104</v>
       </c>
       <c r="K25" s="107" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="L25" s="90"/>
       <c r="M25" s="96"/>
@@ -4489,13 +4489,13 @@
       <c r="O25" s="139"/>
       <c r="P25" s="143"/>
       <c r="Q25" s="93"/>
-      <c r="R25" s="154">
+      <c r="R25" s="148">
         <v>201</v>
       </c>
       <c r="S25" s="94">
         <v>202</v>
       </c>
-      <c r="T25" s="154" t="s">
+      <c r="T25" s="148" t="s">
         <v>334</v>
       </c>
       <c r="U25" s="93"/>
@@ -4684,7 +4684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="33" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A33" s="142"/>
       <c r="B33" s="107"/>
       <c r="C33" s="107"/>
@@ -4710,7 +4710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="34" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A34" s="142"/>
       <c r="B34" s="107"/>
       <c r="C34" s="107"/>
@@ -4736,7 +4736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="35" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A35" s="142"/>
       <c r="B35" s="107"/>
       <c r="C35" s="107"/>
@@ -4762,7 +4762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="36" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A36" s="142"/>
       <c r="B36" s="107"/>
       <c r="C36" s="107"/>
@@ -4788,7 +4788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="37" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A37" s="142"/>
       <c r="B37" s="107"/>
       <c r="C37" s="107"/>
@@ -4814,7 +4814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="38" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A38" s="142"/>
       <c r="B38" s="107"/>
       <c r="C38" s="107"/>
@@ -4840,7 +4840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="39" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A39" s="142"/>
       <c r="B39" s="107"/>
       <c r="C39" s="107"/>
@@ -4866,7 +4866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="40" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A40" s="142"/>
       <c r="B40" s="107"/>
       <c r="C40" s="107"/>
@@ -4892,7 +4892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="10" customFormat="1" ht="11">
+    <row r="41" spans="1:22" s="10" customFormat="1" ht="12">
       <c r="A41" s="142"/>
       <c r="B41" s="107"/>
       <c r="C41" s="107"/>
@@ -7931,7 +7931,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="26">
+    <row r="16" spans="1:5" ht="28">
       <c r="A16" s="127" t="s">
         <v>324</v>
       </c>
@@ -7941,17 +7941,17 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="26">
+    <row r="19" spans="1:1" ht="28">
       <c r="A19" s="127" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="65">
+    <row r="20" spans="1:1" ht="70">
       <c r="A20" s="127" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="39">
+    <row r="21" spans="1:1" ht="42">
       <c r="A21" s="127" t="s">
         <v>284</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="39">
+    <row r="25" spans="1:1" ht="42">
       <c r="A25" s="129" t="s">
         <v>274</v>
       </c>
@@ -7981,27 +7981,27 @@
         <v>305</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="26">
+    <row r="28" spans="1:1" ht="28">
       <c r="A28" s="130" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="26">
+    <row r="29" spans="1:1" ht="28">
       <c r="A29" s="130" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="26">
+    <row r="30" spans="1:1" ht="28">
       <c r="A30" s="130" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="65">
+    <row r="31" spans="1:1" ht="70">
       <c r="A31" s="129" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="26">
+    <row r="32" spans="1:1" ht="28">
       <c r="A32" s="130" t="s">
         <v>286</v>
       </c>
@@ -8013,12 +8013,12 @@
       <c r="C33" s="127"/>
       <c r="E33" s="127"/>
     </row>
-    <row r="34" spans="1:5" ht="26">
+    <row r="34" spans="1:5" ht="28">
       <c r="A34" s="130" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="26">
+    <row r="35" spans="1:5" ht="28">
       <c r="A35" s="129" t="s">
         <v>287</v>
       </c>
@@ -8036,7 +8036,7 @@
       </c>
       <c r="E37" s="127"/>
     </row>
-    <row r="38" spans="1:5" ht="26">
+    <row r="38" spans="1:5" ht="28">
       <c r="A38" s="129" t="s">
         <v>279</v>
       </c>
@@ -8067,12 +8067,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="26">
+    <row r="45" spans="1:5" ht="28">
       <c r="A45" s="129" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="26">
+    <row r="46" spans="1:5" ht="28">
       <c r="A46" s="129" t="s">
         <v>281</v>
       </c>

</xml_diff>

<commit_message>
organism_other is not valid input from OP
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1603.6.microbial.xlsx
+++ b/tests/fixtures/orderforms/1603.6.microbial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C5F137-D9A5-8E49-A1D6-877C9B766283}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEADCFAC-327C-8641-99CA-C0F6919280D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="49600" windowHeight="26740" tabRatio="593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="341">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1457,6 +1457,9 @@
   </si>
   <si>
     <t>optional-fields</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -3547,7 +3550,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3591,7 +3594,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3619,7 +3622,7 @@
   <dimension ref="A1:V151"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -4244,7 +4247,7 @@
         <v>335</v>
       </c>
       <c r="B21" s="107" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="C21" s="107" t="s">
         <v>327</v>
@@ -4304,7 +4307,7 @@
         <v>336</v>
       </c>
       <c r="B22" s="107" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C22" s="107" t="s">
         <v>328</v>
@@ -4352,7 +4355,7 @@
         <v>337</v>
       </c>
       <c r="B23" s="107" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C23" s="107" t="s">
         <v>329</v>
@@ -4404,7 +4407,7 @@
         <v>338</v>
       </c>
       <c r="B24" s="107" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="C24" s="107" t="s">
         <v>332</v>
@@ -4454,7 +4457,7 @@
         <v>339</v>
       </c>
       <c r="B25" s="107" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C25" s="107" t="s">
         <v>333</v>

</xml_diff>

<commit_message>
enabled second family/case analysis pipeline
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1603.6.microbial.xlsx
+++ b/tests/fixtures/orderforms/1603.6.microbial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEADCFAC-327C-8641-99CA-C0F6919280D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08C5508-25EC-3642-B954-1E21F51A6E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="49600" windowHeight="26740" tabRatio="593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3550,7 +3550,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3594,7 +3594,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3622,7 +3622,7 @@
   <dimension ref="A1:V151"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -8178,7 +8178,7 @@
   <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="G1" sqref="G1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>

</xml_diff>